<commit_message>
upd: correct wrong unit for angel
</commit_message>
<xml_diff>
--- a/Raw_Data/DVCS_data/DVCSoutput/5_ALL_PusMstKs.xlsx
+++ b/Raw_Data/DVCS_data/DVCSoutput/5_ALL_PusMstKs.xlsx
@@ -435,7 +435,7 @@
         <v>1.169097942860221</v>
       </c>
       <c r="E1" t="n">
-        <v>0.005265361647294053</v>
+        <v>0.301683</v>
       </c>
       <c r="F1" t="n">
         <v>0.129798</v>
@@ -463,7 +463,7 @@
         <v>1.165975986030587</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01112600274256581</v>
+        <v>0.637473</v>
       </c>
       <c r="F2" t="n">
         <v>-0.0121261</v>
@@ -491,7 +491,7 @@
         <v>1.161145985653828</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01483247120856357</v>
+        <v>0.849838</v>
       </c>
       <c r="F3" t="n">
         <v>-0.0650657</v>
@@ -519,7 +519,7 @@
         <v>1.157648478597886</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01913893151151942</v>
+        <v>1.09658</v>
       </c>
       <c r="F4" t="n">
         <v>0.504813</v>
@@ -547,7 +547,7 @@
         <v>1.160659295400679</v>
       </c>
       <c r="E5" t="n">
-        <v>0.09099151882224797</v>
+        <v>5.21343</v>
       </c>
       <c r="F5" t="n">
         <v>-0.159961</v>
@@ -575,7 +575,7 @@
         <v>1.15959475680084</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0949246182916172</v>
+        <v>5.43878</v>
       </c>
       <c r="F6" t="n">
         <v>-0.124905</v>
@@ -603,7 +603,7 @@
         <v>1.164997854075277</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09888459583146714</v>
+        <v>5.66567</v>
       </c>
       <c r="F7" t="n">
         <v>-0.130172</v>
@@ -631,7 +631,7 @@
         <v>1.170111105835681</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1050107015059672</v>
+        <v>6.01667</v>
       </c>
       <c r="F8" t="n">
         <v>0.119229</v>
@@ -659,7 +659,7 @@
         <v>1.169140710094384</v>
       </c>
       <c r="E9" t="n">
-        <v>0.008706278267600875</v>
+        <v>0.498833</v>
       </c>
       <c r="F9" t="n">
         <v>-0.02502</v>
@@ -687,7 +687,7 @@
         <v>1.162880045404512</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01321933319411529</v>
+        <v>0.757412</v>
       </c>
       <c r="F10" t="n">
         <v>0.196018</v>
@@ -715,7 +715,7 @@
         <v>1.158930541490731</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01697964506753707</v>
+        <v>0.972862</v>
       </c>
       <c r="F11" t="n">
         <v>0.328134</v>
@@ -743,7 +743,7 @@
         <v>1.162471505027112</v>
       </c>
       <c r="E12" t="n">
-        <v>0.09467189461592841</v>
+        <v>5.4243</v>
       </c>
       <c r="F12" t="n">
         <v>-0.167878</v>
@@ -771,7 +771,7 @@
         <v>1.167300304120581</v>
       </c>
       <c r="E13" t="n">
-        <v>0.09861564059373482</v>
+        <v>5.65026</v>
       </c>
       <c r="F13" t="n">
         <v>-0.248583</v>
@@ -799,7 +799,7 @@
         <v>1.259067114970445</v>
       </c>
       <c r="E14" t="n">
-        <v>0.001720931294380701</v>
+        <v>0.0986021</v>
       </c>
       <c r="F14" t="n">
         <v>-0.0606458</v>
@@ -827,7 +827,7 @@
         <v>1.262667810629542</v>
       </c>
       <c r="E15" t="n">
-        <v>0.005034594213595363</v>
+        <v>0.288461</v>
       </c>
       <c r="F15" t="n">
         <v>0.06306929999999999</v>
@@ -855,7 +855,7 @@
         <v>1.2665741194261</v>
       </c>
       <c r="E16" t="n">
-        <v>0.008365258385053701</v>
+        <v>0.479294</v>
       </c>
       <c r="F16" t="n">
         <v>0.180689</v>
@@ -883,7 +883,7 @@
         <v>1.265017786436222</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01147039111056933</v>
+        <v>0.657205</v>
       </c>
       <c r="F17" t="n">
         <v>0.115477</v>
@@ -911,7 +911,7 @@
         <v>1.264045094132326</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01456855997236951</v>
+        <v>0.834717</v>
       </c>
       <c r="F18" t="n">
         <v>0.141207</v>
@@ -939,7 +939,7 @@
         <v>1.260654591868843</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01778804667047581</v>
+        <v>1.01918</v>
       </c>
       <c r="F19" t="n">
         <v>0.0899433</v>
@@ -967,7 +967,7 @@
         <v>1.260749776918481</v>
       </c>
       <c r="E20" t="n">
-        <v>0.03873950261019134</v>
+        <v>2.21961</v>
       </c>
       <c r="F20" t="n">
         <v>0.210126</v>
@@ -995,7 +995,7 @@
         <v>1.251858618215332</v>
       </c>
       <c r="E21" t="n">
-        <v>0.04425858277084781</v>
+        <v>2.53583</v>
       </c>
       <c r="F21" t="n">
         <v>-0.0998786</v>
@@ -1023,7 +1023,7 @@
         <v>1.259118739436436</v>
       </c>
       <c r="E22" t="n">
-        <v>0.05006476959345734</v>
+        <v>2.8685</v>
       </c>
       <c r="F22" t="n">
         <v>0.254379</v>
@@ -1051,7 +1051,7 @@
         <v>1.253973683934396</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05711991402879402</v>
+        <v>3.27273</v>
       </c>
       <c r="F23" t="n">
         <v>0.036488</v>
@@ -1079,7 +1079,7 @@
         <v>1.252449599784359</v>
       </c>
       <c r="E24" t="n">
-        <v>0.09072657784179523</v>
+        <v>5.19825</v>
       </c>
       <c r="F24" t="n">
         <v>-0.20039</v>
@@ -1107,7 +1107,7 @@
         <v>1.259583264417244</v>
       </c>
       <c r="E25" t="n">
-        <v>0.09395456429335876</v>
+        <v>5.3832</v>
       </c>
       <c r="F25" t="n">
         <v>-0.122991</v>
@@ -1135,7 +1135,7 @@
         <v>1.267308170888202</v>
       </c>
       <c r="E26" t="n">
-        <v>0.09704536786571551</v>
+        <v>5.56029</v>
       </c>
       <c r="F26" t="n">
         <v>-0.160578</v>
@@ -1163,7 +1163,7 @@
         <v>1.267497534514367</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1002693400599994</v>
+        <v>5.74501</v>
       </c>
       <c r="F27" t="n">
         <v>-0.240773</v>
@@ -1191,7 +1191,7 @@
         <v>1.262699489189728</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1035034351639449</v>
+        <v>5.93031</v>
       </c>
       <c r="F28" t="n">
         <v>-0.07019830000000001</v>
@@ -1219,7 +1219,7 @@
         <v>1.258348123533388</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1072843419225402</v>
+        <v>6.14694</v>
       </c>
       <c r="F29" t="n">
         <v>-0.0620141</v>
@@ -1247,7 +1247,7 @@
         <v>1.299492208518389</v>
       </c>
       <c r="E30" t="n">
-        <v>0.001701022323603201</v>
+        <v>0.0974614</v>
       </c>
       <c r="F30" t="n">
         <v>0.0732246</v>
@@ -1275,7 +1275,7 @@
         <v>1.299876917250245</v>
       </c>
       <c r="E31" t="n">
-        <v>0.004859171170477412</v>
+        <v>0.27841</v>
       </c>
       <c r="F31" t="n">
         <v>0.0725181</v>
@@ -1303,7 +1303,7 @@
         <v>1.312928025445417</v>
       </c>
       <c r="E32" t="n">
-        <v>0.007834189600256867</v>
+        <v>0.448866</v>
       </c>
       <c r="F32" t="n">
         <v>-0.135158</v>
@@ -1331,7 +1331,7 @@
         <v>1.31040451769673</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0126304591044924</v>
+        <v>0.723672</v>
       </c>
       <c r="F33" t="n">
         <v>0.308131</v>
@@ -1359,7 +1359,7 @@
         <v>1.300342262637034</v>
       </c>
       <c r="E34" t="n">
-        <v>0.02762437326886545</v>
+        <v>1.58276</v>
       </c>
       <c r="F34" t="n">
         <v>0.277034</v>
@@ -1387,7 +1387,7 @@
         <v>1.297100612905568</v>
       </c>
       <c r="E35" t="n">
-        <v>0.03679084250033967</v>
+        <v>2.10796</v>
       </c>
       <c r="F35" t="n">
         <v>0.386755</v>
@@ -1415,7 +1415,7 @@
         <v>1.29490926323044</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0442906968290845</v>
+        <v>2.53767</v>
       </c>
       <c r="F36" t="n">
         <v>0.144717</v>
@@ -1443,7 +1443,7 @@
         <v>1.294758664771161</v>
       </c>
       <c r="E37" t="n">
-        <v>0.05009129859808766</v>
+        <v>2.87002</v>
       </c>
       <c r="F37" t="n">
         <v>-0.0623008</v>
@@ -1471,7 +1471,7 @@
         <v>1.285523239774373</v>
       </c>
       <c r="E38" t="n">
-        <v>0.05915077914641462</v>
+        <v>3.38909</v>
       </c>
       <c r="F38" t="n">
         <v>-0.000776718</v>
@@ -1499,7 +1499,7 @@
         <v>1.321794235121337</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1008004437513813</v>
+        <v>5.77544</v>
       </c>
       <c r="F39" t="n">
         <v>-0.132423</v>
@@ -1527,7 +1527,7 @@
         <v>1.30797171223234</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1047735112606212</v>
+        <v>6.00308</v>
       </c>
       <c r="F40" t="n">
         <v>-0.20428</v>
@@ -1555,7 +1555,7 @@
         <v>1.305181979648815</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1080496687995398</v>
+        <v>6.19079</v>
       </c>
       <c r="F41" t="n">
         <v>0.0735508</v>
@@ -1583,7 +1583,7 @@
         <v>1.304986589969414</v>
       </c>
       <c r="E42" t="n">
-        <v>0.003967098483198071</v>
+        <v>0.227298</v>
       </c>
       <c r="F42" t="n">
         <v>0.279535</v>
@@ -1611,7 +1611,7 @@
         <v>1.309866405401711</v>
       </c>
       <c r="E43" t="n">
-        <v>0.01221587359397367</v>
+        <v>0.699918</v>
       </c>
       <c r="F43" t="n">
         <v>0.261341</v>
@@ -1639,7 +1639,7 @@
         <v>1.311182672246701</v>
       </c>
       <c r="E44" t="n">
-        <v>0.02414069608188477</v>
+        <v>1.38316</v>
       </c>
       <c r="F44" t="n">
         <v>0.620482</v>
@@ -1667,7 +1667,7 @@
         <v>1.303357203532477</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1019319407054492</v>
+        <v>5.84027</v>
       </c>
       <c r="F45" t="n">
         <v>-0.134158</v>
@@ -1695,7 +1695,7 @@
         <v>1.307604680322</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1079512322297273</v>
+        <v>6.18515</v>
       </c>
       <c r="F46" t="n">
         <v>-0.0391029</v>
@@ -1723,7 +1723,7 @@
         <v>1.227774409246259</v>
       </c>
       <c r="E47" t="n">
-        <v>0.004821157899368976</v>
+        <v>0.276232</v>
       </c>
       <c r="F47" t="n">
         <v>0.0553934</v>
@@ -1751,7 +1751,7 @@
         <v>1.256845256982736</v>
       </c>
       <c r="E48" t="n">
-        <v>0.008611646515557741</v>
+        <v>0.493411</v>
       </c>
       <c r="F48" t="n">
         <v>0.144641</v>
@@ -1779,7 +1779,7 @@
         <v>1.267686869853908</v>
       </c>
       <c r="E49" t="n">
-        <v>0.01158444837718716</v>
+        <v>0.66374</v>
       </c>
       <c r="F49" t="n">
         <v>0.178948</v>
@@ -1807,7 +1807,7 @@
         <v>1.263321020168666</v>
       </c>
       <c r="E50" t="n">
-        <v>0.01442907325855012</v>
+        <v>0.826725</v>
       </c>
       <c r="F50" t="n">
         <v>0.0881947</v>
@@ -1835,7 +1835,7 @@
         <v>1.262667810629542</v>
       </c>
       <c r="E51" t="n">
-        <v>0.01759902751248482</v>
+        <v>1.00835</v>
       </c>
       <c r="F51" t="n">
         <v>0.130596</v>
@@ -1863,7 +1863,7 @@
         <v>1.264353589784124</v>
       </c>
       <c r="E52" t="n">
-        <v>0.04223766602996357</v>
+        <v>2.42004</v>
       </c>
       <c r="F52" t="n">
         <v>0.156402</v>
@@ -1891,7 +1891,7 @@
         <v>1.262731166955184</v>
       </c>
       <c r="E53" t="n">
-        <v>0.04665579249846202</v>
+        <v>2.67318</v>
       </c>
       <c r="F53" t="n">
         <v>0.142621</v>
@@ -1919,7 +1919,7 @@
         <v>1.252138171289415</v>
       </c>
       <c r="E54" t="n">
-        <v>0.05022900507607001</v>
+        <v>2.87791</v>
       </c>
       <c r="F54" t="n">
         <v>0.109925</v>
@@ -1947,7 +1947,7 @@
         <v>1.255675117217826</v>
       </c>
       <c r="E55" t="n">
-        <v>0.05578508621686876</v>
+        <v>3.19625</v>
       </c>
       <c r="F55" t="n">
         <v>0.0251794</v>
@@ -1975,7 +1975,7 @@
         <v>1.250967625480372</v>
       </c>
       <c r="E56" t="n">
-        <v>0.09177761511734622</v>
+        <v>5.25847</v>
       </c>
       <c r="F56" t="n">
         <v>-0.233708</v>
@@ -2003,7 +2003,7 @@
         <v>1.262762843925969</v>
       </c>
       <c r="E57" t="n">
-        <v>0.09518414875138875</v>
+        <v>5.45365</v>
       </c>
       <c r="F57" t="n">
         <v>-0.10565</v>
@@ -2031,7 +2031,7 @@
         <v>1.265859391875733</v>
       </c>
       <c r="E58" t="n">
-        <v>0.09805224831119104</v>
+        <v>5.61798</v>
       </c>
       <c r="F58" t="n">
         <v>-0.128623</v>
@@ -2059,7 +2059,7 @@
         <v>1.256924818754089</v>
       </c>
       <c r="E59" t="n">
-        <v>0.1010885976108856</v>
+        <v>5.79195</v>
       </c>
       <c r="F59" t="n">
         <v>-0.100567</v>
@@ -2087,7 +2087,7 @@
         <v>1.225177538155185</v>
       </c>
       <c r="E60" t="n">
-        <v>0.1050993642319685</v>
+        <v>6.02175</v>
       </c>
       <c r="F60" t="n">
         <v>-0.258086</v>
@@ -2115,7 +2115,7 @@
         <v>1.287326687364167</v>
       </c>
       <c r="E61" t="n">
-        <v>0.001623152713696222</v>
+        <v>0.09299979999999999</v>
       </c>
       <c r="F61" t="n">
         <v>-0.0683897</v>
@@ -2143,7 +2143,7 @@
         <v>1.28973253041086</v>
       </c>
       <c r="E62" t="n">
-        <v>0.004941603071049105</v>
+        <v>0.283133</v>
       </c>
       <c r="F62" t="n">
         <v>-0.0164725</v>
@@ -2171,7 +2171,7 @@
         <v>1.305082372879199</v>
       </c>
       <c r="E63" t="n">
-        <v>0.008073491693997809</v>
+        <v>0.462577</v>
       </c>
       <c r="F63" t="n">
         <v>0.257012</v>
@@ -2199,7 +2199,7 @@
         <v>1.317607680609065</v>
       </c>
       <c r="E64" t="n">
-        <v>0.01102126553415363</v>
+        <v>0.631472</v>
       </c>
       <c r="F64" t="n">
         <v>0.6554179999999999</v>
@@ -2227,7 +2227,7 @@
         <v>1.297185414657442</v>
       </c>
       <c r="E65" t="n">
-        <v>0.03842080548877717</v>
+        <v>2.20135</v>
       </c>
       <c r="F65" t="n">
         <v>0.135683</v>
@@ -2255,7 +2255,7 @@
         <v>1.292068109659859</v>
       </c>
       <c r="E66" t="n">
-        <v>0.04492442588048365</v>
+        <v>2.57398</v>
       </c>
       <c r="F66" t="n">
         <v>-0.08765870000000001</v>
@@ -2283,7 +2283,7 @@
         <v>1.295430430397557</v>
       </c>
       <c r="E67" t="n">
-        <v>0.04941184192028627</v>
+        <v>2.83109</v>
       </c>
       <c r="F67" t="n">
         <v>0.0396971</v>
@@ -2311,7 +2311,7 @@
         <v>1.287998447204033</v>
       </c>
       <c r="E68" t="n">
-        <v>0.05353622947567407</v>
+        <v>3.0674</v>
       </c>
       <c r="F68" t="n">
         <v>-0.072587</v>
@@ -2339,7 +2339,7 @@
         <v>1.28825851442946</v>
       </c>
       <c r="E69" t="n">
-        <v>0.06018471219529607</v>
+        <v>3.44833</v>
       </c>
       <c r="F69" t="n">
         <v>-0.336625</v>
@@ -2367,7 +2367,7 @@
         <v>1.313270726088113</v>
       </c>
       <c r="E70" t="n">
-        <v>0.09971013656766045</v>
+        <v>5.71297</v>
       </c>
       <c r="F70" t="n">
         <v>-0.327082</v>
@@ -2395,7 +2395,7 @@
         <v>1.297601633784422</v>
       </c>
       <c r="E71" t="n">
-        <v>0.1025620045654192</v>
+        <v>5.87637</v>
       </c>
       <c r="F71" t="n">
         <v>-0.0402555</v>
@@ -2423,7 +2423,7 @@
         <v>1.288328374289723</v>
       </c>
       <c r="E72" t="n">
-        <v>0.1067787200382375</v>
+        <v>6.11797</v>
       </c>
       <c r="F72" t="n">
         <v>-0.0280145</v>
@@ -2451,7 +2451,7 @@
         <v>1.248647268046505</v>
       </c>
       <c r="E73" t="n">
-        <v>0.007884943774904863</v>
+        <v>0.451774</v>
       </c>
       <c r="F73" t="n">
         <v>0.163241</v>
@@ -2479,7 +2479,7 @@
         <v>1.264104426066138</v>
       </c>
       <c r="E74" t="n">
-        <v>0.01048925427156072</v>
+        <v>0.60099</v>
       </c>
       <c r="F74" t="n">
         <v>0.142182</v>
@@ -2507,7 +2507,7 @@
         <v>1.269818884723329</v>
       </c>
       <c r="E75" t="n">
-        <v>0.01330848461230716</v>
+        <v>0.76252</v>
       </c>
       <c r="F75" t="n">
         <v>0.172023</v>
@@ -2535,7 +2535,7 @@
         <v>1.27443713065808</v>
       </c>
       <c r="E76" t="n">
-        <v>0.04440327056583813</v>
+        <v>2.54412</v>
       </c>
       <c r="F76" t="n">
         <v>0.374767</v>
@@ -2563,7 +2563,7 @@
         <v>1.242642345970875</v>
       </c>
       <c r="E77" t="n">
-        <v>0.05236842967316466</v>
+        <v>3.00049</v>
       </c>
       <c r="F77" t="n">
         <v>-0.137749</v>
@@ -2591,7 +2591,7 @@
         <v>1.254360394782935</v>
       </c>
       <c r="E78" t="n">
-        <v>0.07743292852813002</v>
+        <v>4.43658</v>
       </c>
       <c r="F78" t="n">
         <v>0.2065</v>
@@ -2619,7 +2619,7 @@
         <v>1.247132711462577</v>
       </c>
       <c r="E79" t="n">
-        <v>0.08348293784724317</v>
+        <v>4.78322</v>
       </c>
       <c r="F79" t="n">
         <v>-0.142873</v>
@@ -2647,7 +2647,7 @@
         <v>1.260285681899148</v>
       </c>
       <c r="E80" t="n">
-        <v>0.09408336959215592</v>
+        <v>5.39058</v>
       </c>
       <c r="F80" t="n">
         <v>0.0935139</v>
@@ -2675,7 +2675,7 @@
         <v>1.262865788593546</v>
       </c>
       <c r="E81" t="n">
-        <v>0.09842278171138943</v>
+        <v>5.63921</v>
       </c>
       <c r="F81" t="n">
         <v>-0.262938</v>
@@ -2703,7 +2703,7 @@
         <v>1.24853914636266</v>
       </c>
       <c r="E82" t="n">
-        <v>0.1009688680241988</v>
+        <v>5.78509</v>
       </c>
       <c r="F82" t="n">
         <v>-0.0620986</v>
@@ -2731,7 +2731,7 @@
         <v>1.293916535175279</v>
       </c>
       <c r="E83" t="n">
-        <v>0.003130876331982548</v>
+        <v>0.179386</v>
       </c>
       <c r="F83" t="n">
         <v>0.0220792</v>
@@ -2759,7 +2759,7 @@
         <v>1.286670120893463</v>
       </c>
       <c r="E84" t="n">
-        <v>0.007269732666869381</v>
+        <v>0.416525</v>
       </c>
       <c r="F84" t="n">
         <v>0.000613912</v>
@@ -2787,7 +2787,7 @@
         <v>1.306770829181613</v>
       </c>
       <c r="E85" t="n">
-        <v>0.009838263913859358</v>
+        <v>0.5636910000000001</v>
       </c>
       <c r="F85" t="n">
         <v>0.197259</v>
@@ -2815,7 +2815,7 @@
         <v>1.295758465146958</v>
       </c>
       <c r="E86" t="n">
-        <v>0.04134911890777326</v>
+        <v>2.36913</v>
       </c>
       <c r="F86" t="n">
         <v>0.0275525</v>
@@ -2843,7 +2843,7 @@
         <v>1.289317648991124</v>
       </c>
       <c r="E87" t="n">
-        <v>0.04948340041961803</v>
+        <v>2.83519</v>
       </c>
       <c r="F87" t="n">
         <v>-0.0320458</v>
@@ -2871,7 +2871,7 @@
         <v>1.289561941125745</v>
       </c>
       <c r="E88" t="n">
-        <v>0.05873748517954236</v>
+        <v>3.36541</v>
       </c>
       <c r="F88" t="n">
         <v>0.0476292</v>
@@ -2899,7 +2899,7 @@
         <v>1.299091990584193</v>
       </c>
       <c r="E89" t="n">
-        <v>0.08361087048141434</v>
+        <v>4.79055</v>
       </c>
       <c r="F89" t="n">
         <v>-0.166888</v>
@@ -2927,7 +2927,7 @@
         <v>1.287489805784885</v>
       </c>
       <c r="E90" t="n">
-        <v>0.09016231289462547</v>
+        <v>5.16592</v>
       </c>
       <c r="F90" t="n">
         <v>-0.0637423</v>
@@ -2955,7 +2955,7 @@
         <v>1.304338913013025</v>
       </c>
       <c r="E91" t="n">
-        <v>0.09911480475980519</v>
+        <v>5.67886</v>
       </c>
       <c r="F91" t="n">
         <v>-0.336356</v>
@@ -2983,7 +2983,7 @@
         <v>1.28970151585551</v>
       </c>
       <c r="E92" t="n">
-        <v>0.1024103354534209</v>
+        <v>5.86768</v>
       </c>
       <c r="F92" t="n">
         <v>-0.0152803</v>
@@ -3011,7 +3011,7 @@
         <v>1.29238539143709</v>
       </c>
       <c r="E93" t="n">
-        <v>0.1062104408337881</v>
+        <v>6.08541</v>
       </c>
       <c r="F93" t="n">
         <v>0.0542667</v>
@@ -3039,7 +3039,7 @@
         <v>1.254691197068027</v>
       </c>
       <c r="E94" t="n">
-        <v>0.002127364371963368</v>
+        <v>0.121889</v>
       </c>
       <c r="F94" t="n">
         <v>0.198784</v>
@@ -3067,7 +3067,7 @@
         <v>1.261372268602731</v>
       </c>
       <c r="E95" t="n">
-        <v>0.006321634910601021</v>
+        <v>0.362203</v>
       </c>
       <c r="F95" t="n">
         <v>-0.09295299999999999</v>
@@ -3095,7 +3095,7 @@
         <v>1.270444803995829</v>
       </c>
       <c r="E96" t="n">
-        <v>0.1014915941351711</v>
+        <v>5.81504</v>
       </c>
       <c r="F96" t="n">
         <v>-0.121317</v>
@@ -3123,7 +3123,7 @@
         <v>1.25425675202488</v>
       </c>
       <c r="E97" t="n">
-        <v>0.1044799468804357</v>
+        <v>5.98626</v>
       </c>
       <c r="F97" t="n">
         <v>0.117809</v>
@@ -3151,7 +3151,7 @@
         <v>1.260587164776796</v>
       </c>
       <c r="E98" t="n">
-        <v>0.1080259323217126</v>
+        <v>6.18943</v>
       </c>
       <c r="F98" t="n">
         <v>0.0558603</v>
@@ -3179,7 +3179,7 @@
         <v>1.422462653288303</v>
       </c>
       <c r="E99" t="n">
-        <v>0.001681722472734648</v>
+        <v>0.0963556</v>
       </c>
       <c r="F99" t="n">
         <v>0.0144519</v>
@@ -3207,7 +3207,7 @@
         <v>1.425692814038143</v>
       </c>
       <c r="E100" t="n">
-        <v>0.005026583152328709</v>
+        <v>0.288002</v>
       </c>
       <c r="F100" t="n">
         <v>0.0785324</v>
@@ -3235,7 +3235,7 @@
         <v>1.428940166696982</v>
       </c>
       <c r="E101" t="n">
-        <v>0.008248391138340161</v>
+        <v>0.472598</v>
       </c>
       <c r="F101" t="n">
         <v>0.130264</v>
@@ -3263,7 +3263,7 @@
         <v>1.423534333973017</v>
       </c>
       <c r="E102" t="n">
-        <v>0.01135022519156952</v>
+        <v>0.65032</v>
       </c>
       <c r="F102" t="n">
         <v>0.106946</v>
@@ -3291,7 +3291,7 @@
         <v>1.421084093218976</v>
       </c>
       <c r="E103" t="n">
-        <v>0.01445401401356112</v>
+        <v>0.8281539999999999</v>
       </c>
       <c r="F103" t="n">
         <v>0.329336</v>
@@ -3319,7 +3319,7 @@
         <v>1.40965243943321</v>
       </c>
       <c r="E104" t="n">
-        <v>0.01811477230644915</v>
+        <v>1.0379</v>
       </c>
       <c r="F104" t="n">
         <v>-0.272546</v>
@@ -3347,7 +3347,7 @@
         <v>1.410553083013893</v>
       </c>
       <c r="E105" t="n">
-        <v>0.03421176946466765</v>
+        <v>1.96019</v>
       </c>
       <c r="F105" t="n">
         <v>0.24106</v>
@@ -3375,7 +3375,7 @@
         <v>1.414146385633397</v>
       </c>
       <c r="E106" t="n">
-        <v>0.04126359777442554</v>
+        <v>2.36423</v>
       </c>
       <c r="F106" t="n">
         <v>0.108634</v>
@@ -3403,7 +3403,7 @@
         <v>1.406719588261996</v>
       </c>
       <c r="E107" t="n">
-        <v>0.04762654462842127</v>
+        <v>2.7288</v>
       </c>
       <c r="F107" t="n">
         <v>0.266575</v>
@@ -3431,7 +3431,7 @@
         <v>1.408655387239903</v>
       </c>
       <c r="E108" t="n">
-        <v>0.0558653713624605</v>
+        <v>3.20085</v>
       </c>
       <c r="F108" t="n">
         <v>0.0349802</v>
@@ -3459,7 +3459,7 @@
         <v>1.40922319027186</v>
       </c>
       <c r="E109" t="n">
-        <v>0.06418291244576467</v>
+        <v>3.67741</v>
       </c>
       <c r="F109" t="n">
         <v>-0.127259</v>
@@ -3487,7 +3487,7 @@
         <v>1.390855851625178</v>
       </c>
       <c r="E110" t="n">
-        <v>0.09186749957382394</v>
+        <v>5.26362</v>
       </c>
       <c r="F110" t="n">
         <v>-0.0170134</v>
@@ -3515,7 +3515,7 @@
         <v>1.415902539018841</v>
       </c>
       <c r="E111" t="n">
-        <v>0.09516058680648683</v>
+        <v>5.4523</v>
       </c>
       <c r="F111" t="n">
         <v>-0.294424</v>
@@ -3543,7 +3543,7 @@
         <v>1.423983848223006</v>
       </c>
       <c r="E112" t="n">
-        <v>0.09823969667285523</v>
+        <v>5.62872</v>
       </c>
       <c r="F112" t="n">
         <v>-0.0965065</v>
@@ -3571,7 +3571,7 @@
         <v>1.429006647990134</v>
       </c>
       <c r="E113" t="n">
-        <v>0.101392633966583</v>
+        <v>5.80937</v>
       </c>
       <c r="F113" t="n">
         <v>-0.106931</v>
@@ -3599,7 +3599,7 @@
         <v>1.422431017659556</v>
       </c>
       <c r="E114" t="n">
-        <v>0.1046096248438589</v>
+        <v>5.99369</v>
       </c>
       <c r="F114" t="n">
         <v>-0.0187838</v>
@@ -3627,7 +3627,7 @@
         <v>1.42256810030311</v>
       </c>
       <c r="E115" t="n">
-        <v>0.1079671147259204</v>
+        <v>6.18606</v>
       </c>
       <c r="F115" t="n">
         <v>-0.09558990000000001</v>
@@ -3655,7 +3655,7 @@
         <v>1.479111219618052</v>
       </c>
       <c r="E116" t="n">
-        <v>0.001640871296262469</v>
+        <v>0.094015</v>
       </c>
       <c r="F116" t="n">
         <v>0.00293917</v>
@@ -3683,7 +3683,7 @@
         <v>1.469938774235172</v>
       </c>
       <c r="E117" t="n">
-        <v>0.004911181982186844</v>
+        <v>0.28139</v>
       </c>
       <c r="F117" t="n">
         <v>0.008042550000000001</v>
@@ -3711,7 +3711,7 @@
         <v>1.473475483338627</v>
       </c>
       <c r="E118" t="n">
-        <v>0.008123041591461929</v>
+        <v>0.465416</v>
       </c>
       <c r="F118" t="n">
         <v>0.2125</v>
@@ -3739,7 +3739,7 @@
         <v>1.46171132580958</v>
       </c>
       <c r="E119" t="n">
-        <v>0.01141981146884654</v>
+        <v>0.654307</v>
       </c>
       <c r="F119" t="n">
         <v>0.242538</v>
@@ -3767,7 +3767,7 @@
         <v>1.457988340145421</v>
       </c>
       <c r="E120" t="n">
-        <v>0.01473101521914514</v>
+        <v>0.844025</v>
       </c>
       <c r="F120" t="n">
         <v>0.28868</v>
@@ -3795,7 +3795,7 @@
         <v>1.461906289746371</v>
       </c>
       <c r="E121" t="n">
-        <v>0.01814287210740625</v>
+        <v>1.03951</v>
       </c>
       <c r="F121" t="n">
         <v>0.0712511</v>
@@ -3823,7 +3823,7 @@
         <v>1.463123371421563</v>
       </c>
       <c r="E122" t="n">
-        <v>0.02206445240371232</v>
+        <v>1.2642</v>
       </c>
       <c r="F122" t="n">
         <v>0.42536</v>
@@ -3851,7 +3851,7 @@
         <v>1.454737089648848</v>
       </c>
       <c r="E123" t="n">
-        <v>0.0261921560846789</v>
+        <v>1.5007</v>
       </c>
       <c r="F123" t="n">
         <v>0.451736</v>
@@ -3879,7 +3879,7 @@
         <v>1.459184703867197</v>
       </c>
       <c r="E124" t="n">
-        <v>0.03011146745295737</v>
+        <v>1.72526</v>
       </c>
       <c r="F124" t="n">
         <v>0.214882</v>
@@ -3907,7 +3907,7 @@
         <v>1.456111259485346</v>
       </c>
       <c r="E125" t="n">
-        <v>0.03341485212820704</v>
+        <v>1.91453</v>
       </c>
       <c r="F125" t="n">
         <v>0.200965</v>
@@ -3935,7 +3935,7 @@
         <v>1.455596097823843</v>
       </c>
       <c r="E126" t="n">
-        <v>0.03726085966790174</v>
+        <v>2.13489</v>
       </c>
       <c r="F126" t="n">
         <v>0.333614</v>
@@ -3963,7 +3963,7 @@
         <v>1.449651682301649</v>
       </c>
       <c r="E127" t="n">
-        <v>0.0410576489226902</v>
+        <v>2.35243</v>
       </c>
       <c r="F127" t="n">
         <v>0.0383853</v>
@@ -3991,7 +3991,7 @@
         <v>1.463482148849107</v>
       </c>
       <c r="E128" t="n">
-        <v>0.04500942341505577</v>
+        <v>2.57885</v>
       </c>
       <c r="F128" t="n">
         <v>0.0736695</v>
@@ -4019,7 +4019,7 @@
         <v>1.459832182136015</v>
       </c>
       <c r="E129" t="n">
-        <v>0.0502639116611099</v>
+        <v>2.87991</v>
       </c>
       <c r="F129" t="n">
         <v>0.160882</v>
@@ -4047,7 +4047,7 @@
         <v>1.459153864402243</v>
       </c>
       <c r="E130" t="n">
-        <v>0.05829033182518142</v>
+        <v>3.33979</v>
       </c>
       <c r="F130" t="n">
         <v>-0.09413059999999999</v>
@@ -4075,7 +4075,7 @@
         <v>1.463567559082942</v>
       </c>
       <c r="E131" t="n">
-        <v>0.0674386496324349</v>
+        <v>3.86395</v>
       </c>
       <c r="F131" t="n">
         <v>-0.304386</v>
@@ -4103,7 +4103,7 @@
         <v>1.474588078074687</v>
       </c>
       <c r="E132" t="n">
-        <v>0.07786803911065221</v>
+        <v>4.46151</v>
       </c>
       <c r="F132" t="n">
         <v>-0.21955</v>
@@ -4131,7 +4131,7 @@
         <v>1.500809781418018</v>
       </c>
       <c r="E133" t="n">
-        <v>0.09880221629077299</v>
+        <v>5.66095</v>
       </c>
       <c r="F133" t="n">
         <v>-0.0221449</v>
@@ -4159,7 +4159,7 @@
         <v>1.491331619727819</v>
       </c>
       <c r="E134" t="n">
-        <v>0.1027323487004138</v>
+        <v>5.88613</v>
       </c>
       <c r="F134" t="n">
         <v>0.0447147</v>
@@ -4187,7 +4187,7 @@
         <v>1.486112377984922</v>
       </c>
       <c r="E135" t="n">
-        <v>0.1070787421366553</v>
+        <v>6.13516</v>
       </c>
       <c r="F135" t="n">
         <v>-0.00338804</v>
@@ -4215,7 +4215,7 @@
         <v>1.469265122433661</v>
       </c>
       <c r="E136" t="n">
-        <v>0.001718274903259165</v>
+        <v>0.09844990000000001</v>
       </c>
       <c r="F136" t="n">
         <v>0.0552195</v>
@@ -4243,7 +4243,7 @@
         <v>1.46365638043907</v>
       </c>
       <c r="E137" t="n">
-        <v>0.004837843247018042</v>
+        <v>0.277188</v>
       </c>
       <c r="F137" t="n">
         <v>0.0539578</v>
@@ -4271,7 +4271,7 @@
         <v>1.465776244861404</v>
       </c>
       <c r="E138" t="n">
-        <v>0.008377318610184982</v>
+        <v>0.479985</v>
       </c>
       <c r="F138" t="n">
         <v>0.0413396</v>
@@ -4299,7 +4299,7 @@
         <v>1.459787655791074</v>
       </c>
       <c r="E139" t="n">
-        <v>0.01178762215541182</v>
+        <v>0.675381</v>
       </c>
       <c r="F139" t="n">
         <v>0.313602</v>
@@ -4327,7 +4327,7 @@
         <v>1.45511511572109</v>
       </c>
       <c r="E140" t="n">
-        <v>0.01637542953378916</v>
+        <v>0.938243</v>
       </c>
       <c r="F140" t="n">
         <v>0.103809</v>
@@ -4355,7 +4355,7 @@
         <v>1.468734148850635</v>
       </c>
       <c r="E141" t="n">
-        <v>0.02318059046036269</v>
+        <v>1.32815</v>
       </c>
       <c r="F141" t="n">
         <v>0.466141</v>
@@ -4383,7 +4383,7 @@
         <v>1.467865797680428</v>
       </c>
       <c r="E142" t="n">
-        <v>0.09057438513102134</v>
+        <v>5.18953</v>
       </c>
       <c r="F142" t="n">
         <v>-0.0434758</v>
@@ -4411,7 +4411,7 @@
         <v>1.479263330174854</v>
       </c>
       <c r="E143" t="n">
-        <v>0.09839171485070393</v>
+        <v>5.63743</v>
       </c>
       <c r="F143" t="n">
         <v>-0.162394</v>
@@ -4439,7 +4439,7 @@
         <v>1.461358956588011</v>
       </c>
       <c r="E144" t="n">
-        <v>0.102481370353977</v>
+        <v>5.87175</v>
       </c>
       <c r="F144" t="n">
         <v>0.159152</v>
@@ -4467,7 +4467,7 @@
         <v>1.466315109381336</v>
       </c>
       <c r="E145" t="n">
-        <v>0.107116092182648</v>
+        <v>6.1373</v>
       </c>
       <c r="F145" t="n">
         <v>-0.073077</v>
@@ -4495,7 +4495,7 @@
         <v>1.382794272478737</v>
       </c>
       <c r="E146" t="n">
-        <v>0.001763428316337511</v>
+        <v>0.101037</v>
       </c>
       <c r="F146" t="n">
         <v>-0.033155</v>
@@ -4523,7 +4523,7 @@
         <v>1.396449068172556</v>
       </c>
       <c r="E147" t="n">
-        <v>0.005172492677795435</v>
+        <v>0.296362</v>
       </c>
       <c r="F147" t="n">
         <v>0.0437502</v>
@@ -4551,7 +4551,7 @@
         <v>1.41709562133259</v>
       </c>
       <c r="E148" t="n">
-        <v>0.008344855486097889</v>
+        <v>0.478125</v>
       </c>
       <c r="F148" t="n">
         <v>0.0712709</v>
@@ -4579,7 +4579,7 @@
         <v>1.4264431289049</v>
       </c>
       <c r="E149" t="n">
-        <v>0.01142181859748633</v>
+        <v>0.6544219999999999</v>
       </c>
       <c r="F149" t="n">
         <v>0.160004</v>
@@ -4607,7 +4607,7 @@
         <v>1.423168999100247</v>
       </c>
       <c r="E150" t="n">
-        <v>0.01437420010686742</v>
+        <v>0.823581</v>
       </c>
       <c r="F150" t="n">
         <v>0.179854</v>
@@ -4635,7 +4635,7 @@
         <v>1.420609024327243</v>
       </c>
       <c r="E151" t="n">
-        <v>0.03483869173198401</v>
+        <v>1.99611</v>
       </c>
       <c r="F151" t="n">
         <v>-0.0053057</v>
@@ -4663,7 +4663,7 @@
         <v>1.417176770907568</v>
       </c>
       <c r="E152" t="n">
-        <v>0.04149625016371638</v>
+        <v>2.37756</v>
       </c>
       <c r="F152" t="n">
         <v>0.387993</v>
@@ -4691,7 +4691,7 @@
         <v>1.41091105318514</v>
       </c>
       <c r="E153" t="n">
-        <v>0.046661028486218</v>
+        <v>2.67348</v>
       </c>
       <c r="F153" t="n">
         <v>0.0212293</v>
@@ -4719,7 +4719,7 @@
         <v>1.406132995132395</v>
       </c>
       <c r="E154" t="n">
-        <v>0.05060721792497717</v>
+        <v>2.89958</v>
       </c>
       <c r="F154" t="n">
         <v>0.0517483</v>
@@ -4747,7 +4747,7 @@
         <v>1.419327305451424</v>
       </c>
       <c r="E155" t="n">
-        <v>0.05585263045892094</v>
+        <v>3.20012</v>
       </c>
       <c r="F155" t="n">
         <v>-0.0564642</v>
@@ -4775,7 +4775,7 @@
         <v>1.41725791583607</v>
       </c>
       <c r="E156" t="n">
-        <v>0.078055138406466</v>
+        <v>4.47223</v>
       </c>
       <c r="F156" t="n">
         <v>-0.773884</v>
@@ -4803,7 +4803,7 @@
         <v>1.426281879573599</v>
       </c>
       <c r="E157" t="n">
-        <v>0.09513597766403371</v>
+        <v>5.45089</v>
       </c>
       <c r="F157" t="n">
         <v>-0.188897</v>
@@ -4831,7 +4831,7 @@
         <v>1.42638704424851</v>
       </c>
       <c r="E158" t="n">
-        <v>0.09824196560088282</v>
+        <v>5.62885</v>
       </c>
       <c r="F158" t="n">
         <v>-0.126506</v>
@@ -4859,7 +4859,7 @@
         <v>1.413088815326199</v>
       </c>
       <c r="E159" t="n">
-        <v>0.1013416703524248</v>
+        <v>5.80645</v>
       </c>
       <c r="F159" t="n">
         <v>-0.172939</v>
@@ -4887,7 +4887,7 @@
         <v>1.395646803457092</v>
       </c>
       <c r="E160" t="n">
-        <v>0.1044960039095541</v>
+        <v>5.98718</v>
       </c>
       <c r="F160" t="n">
         <v>-0.101704</v>
@@ -4915,7 +4915,7 @@
         <v>1.382432638503591</v>
       </c>
       <c r="E161" t="n">
-        <v>0.107779491831331</v>
+        <v>6.17531</v>
       </c>
       <c r="F161" t="n">
         <v>-0.11134</v>
@@ -4943,7 +4943,7 @@
         <v>1.462716650619661</v>
       </c>
       <c r="E162" t="n">
-        <v>0.001649252367330546</v>
+        <v>0.0944952</v>
       </c>
       <c r="F162" t="n">
         <v>0.0621024</v>
@@ -4971,7 +4971,7 @@
         <v>1.467000340831589</v>
       </c>
       <c r="E163" t="n">
-        <v>0.004909017773914371</v>
+        <v>0.281266</v>
       </c>
       <c r="F163" t="n">
         <v>0.0659078</v>
@@ -4999,7 +4999,7 @@
         <v>1.494583554037713</v>
       </c>
       <c r="E164" t="n">
-        <v>0.008035443516304334</v>
+        <v>0.460397</v>
       </c>
       <c r="F164" t="n">
         <v>0.20115</v>
@@ -5027,7 +5027,7 @@
         <v>1.509937084782012</v>
       </c>
       <c r="E165" t="n">
-        <v>0.01099899513289818</v>
+        <v>0.630196</v>
       </c>
       <c r="F165" t="n">
         <v>0.200399</v>
@@ -5055,7 +5055,7 @@
         <v>1.487948251788348</v>
       </c>
       <c r="E166" t="n">
-        <v>0.01897329976550515</v>
+        <v>1.08709</v>
       </c>
       <c r="F166" t="n">
         <v>0.176808</v>
@@ -5083,7 +5083,7 @@
         <v>1.468972429965927</v>
       </c>
       <c r="E167" t="n">
-        <v>0.02782875132427399</v>
+        <v>1.59447</v>
       </c>
       <c r="F167" t="n">
         <v>0.294433</v>
@@ -5111,7 +5111,7 @@
         <v>1.456403103539676</v>
       </c>
       <c r="E168" t="n">
-        <v>0.0328413369360017</v>
+        <v>1.88167</v>
       </c>
       <c r="F168" t="n">
         <v>0.249741</v>
@@ -5139,7 +5139,7 @@
         <v>1.450827350169551</v>
       </c>
       <c r="E169" t="n">
-        <v>0.03719994767700714</v>
+        <v>2.1314</v>
       </c>
       <c r="F169" t="n">
         <v>0.199409</v>
@@ -5167,7 +5167,7 @@
         <v>1.459424544126896</v>
       </c>
       <c r="E170" t="n">
-        <v>0.04123689423687002</v>
+        <v>2.3627</v>
       </c>
       <c r="F170" t="n">
         <v>-0.201706</v>
@@ -5195,7 +5195,7 @@
         <v>1.453660895807547</v>
       </c>
       <c r="E171" t="n">
-        <v>0.04445964470067755</v>
+        <v>2.54735</v>
       </c>
       <c r="F171" t="n">
         <v>0.057878</v>
@@ -5223,7 +5223,7 @@
         <v>1.455067008766263</v>
       </c>
       <c r="E172" t="n">
-        <v>0.04756859969725506</v>
+        <v>2.72548</v>
       </c>
       <c r="F172" t="n">
         <v>0.0113838</v>
@@ -5251,7 +5251,7 @@
         <v>1.449899996551486</v>
       </c>
       <c r="E173" t="n">
-        <v>0.05090287670026502</v>
+        <v>2.91652</v>
       </c>
       <c r="F173" t="n">
         <v>0.00427523</v>
@@ -5279,7 +5279,7 @@
         <v>1.45033444418865</v>
       </c>
       <c r="E174" t="n">
-        <v>0.05456213400999634</v>
+        <v>3.12618</v>
       </c>
       <c r="F174" t="n">
         <v>0.159279</v>
@@ -5307,7 +5307,7 @@
         <v>1.440531152040802</v>
       </c>
       <c r="E175" t="n">
-        <v>0.05919423784478928</v>
+        <v>3.39158</v>
       </c>
       <c r="F175" t="n">
         <v>0.0257898</v>
@@ -5335,7 +5335,7 @@
         <v>1.450665364582749</v>
       </c>
       <c r="E176" t="n">
-        <v>0.06358810423668501</v>
+        <v>3.64333</v>
       </c>
       <c r="F176" t="n">
         <v>0.175598</v>
@@ -5363,7 +5363,7 @@
         <v>1.462843122142631</v>
       </c>
       <c r="E177" t="n">
-        <v>0.06925902804226498</v>
+        <v>3.96825</v>
       </c>
       <c r="F177" t="n">
         <v>-0.0598139</v>
@@ -5391,7 +5391,7 @@
         <v>1.479689156546063</v>
       </c>
       <c r="E178" t="n">
-        <v>0.08136864599137723</v>
+        <v>4.66208</v>
       </c>
       <c r="F178" t="n">
         <v>-0.37776</v>
@@ -5419,7 +5419,7 @@
         <v>1.502800718658332</v>
       </c>
       <c r="E179" t="n">
-        <v>0.09319325167363882</v>
+        <v>5.33958</v>
       </c>
       <c r="F179" t="n">
         <v>-0.149014</v>
@@ -5447,7 +5447,7 @@
         <v>1.512299573497262</v>
       </c>
       <c r="E180" t="n">
-        <v>0.09952600433157505</v>
+        <v>5.70242</v>
       </c>
       <c r="F180" t="n">
         <v>-0.347884</v>
@@ -5475,7 +5475,7 @@
         <v>1.489123903508368</v>
       </c>
       <c r="E181" t="n">
-        <v>0.1026129681795774</v>
+        <v>5.87929</v>
       </c>
       <c r="F181" t="n">
         <v>-0.127391</v>
@@ -5503,7 +5503,7 @@
         <v>1.463256641877972</v>
       </c>
       <c r="E182" t="n">
-        <v>0.1069501113707833</v>
+        <v>6.12779</v>
       </c>
       <c r="F182" t="n">
         <v>-0.0341788</v>
@@ -5531,7 +5531,7 @@
         <v>1.459592408859405</v>
       </c>
       <c r="E183" t="n">
-        <v>0.001547478727988252</v>
+        <v>0.08866400000000001</v>
       </c>
       <c r="F183" t="n">
         <v>0.0756978</v>
@@ -5559,7 +5559,7 @@
         <v>1.471872956474165</v>
       </c>
       <c r="E184" t="n">
-        <v>0.005263005452803861</v>
+        <v>0.301548</v>
       </c>
       <c r="F184" t="n">
         <v>0.0478776</v>
@@ -5587,7 +5587,7 @@
         <v>1.479949323456719</v>
       </c>
       <c r="E185" t="n">
-        <v>0.01278179660393283</v>
+        <v>0.732343</v>
       </c>
       <c r="F185" t="n">
         <v>0.3544</v>
@@ -5615,7 +5615,7 @@
         <v>1.477260978974264</v>
       </c>
       <c r="E186" t="n">
-        <v>0.02438940550029396</v>
+        <v>1.39741</v>
       </c>
       <c r="F186" t="n">
         <v>0.38048</v>
@@ -5643,7 +5643,7 @@
         <v>1.454248947051364</v>
       </c>
       <c r="E187" t="n">
-        <v>0.03580961839486846</v>
+        <v>2.05174</v>
       </c>
       <c r="F187" t="n">
         <v>-0.163878</v>
@@ -5671,7 +5671,7 @@
         <v>1.467416096408922</v>
       </c>
       <c r="E188" t="n">
-        <v>0.04534417756558828</v>
+        <v>2.59803</v>
       </c>
       <c r="F188" t="n">
         <v>0.0435184</v>
@@ -5699,7 +5699,7 @@
         <v>1.474411747104587</v>
       </c>
       <c r="E189" t="n">
-        <v>0.05639542785629117</v>
+        <v>3.23122</v>
       </c>
       <c r="F189" t="n">
         <v>-0.344274</v>
@@ -5727,7 +5727,7 @@
         <v>1.461324741458927</v>
       </c>
       <c r="E190" t="n">
-        <v>0.06814917317092178</v>
+        <v>3.90466</v>
       </c>
       <c r="F190" t="n">
         <v>-0.55406</v>
@@ -5755,7 +5755,7 @@
         <v>1.48094902005437</v>
       </c>
       <c r="E191" t="n">
-        <v>0.1029286982412632</v>
+        <v>5.89738</v>
       </c>
       <c r="F191" t="n">
         <v>-0.195411</v>
@@ -5783,7 +5783,7 @@
         <v>1.458903697986951</v>
       </c>
       <c r="E192" t="n">
-        <v>0.1080395458898782</v>
+        <v>6.19021</v>
       </c>
       <c r="F192" t="n">
         <v>-0.06312280000000001</v>
@@ -5811,7 +5811,7 @@
         <v>1.394184349359869</v>
       </c>
       <c r="E193" t="n">
-        <v>0.007823665264867342</v>
+        <v>0.448263</v>
       </c>
       <c r="F193" t="n">
         <v>0.0485477</v>
@@ -5839,7 +5839,7 @@
         <v>1.42072868627335</v>
       </c>
       <c r="E194" t="n">
-        <v>0.01036795388854712</v>
+        <v>0.59404</v>
       </c>
       <c r="F194" t="n">
         <v>0.13168</v>
@@ -5867,7 +5867,7 @@
         <v>1.423576481963649</v>
       </c>
       <c r="E195" t="n">
-        <v>0.01322926411755914</v>
+        <v>0.757981</v>
       </c>
       <c r="F195" t="n">
         <v>0.21003</v>
@@ -5895,7 +5895,7 @@
         <v>1.409631157430907</v>
       </c>
       <c r="E196" t="n">
-        <v>0.04310893439255914</v>
+        <v>2.46996</v>
       </c>
       <c r="F196" t="n">
         <v>0.107849</v>
@@ -5923,7 +5923,7 @@
         <v>1.411247674931654</v>
       </c>
       <c r="E197" t="n">
-        <v>0.0506649883232182</v>
+        <v>2.90289</v>
       </c>
       <c r="F197" t="n">
         <v>0.0599243</v>
@@ -5951,7 +5951,7 @@
         <v>1.405097861360553</v>
       </c>
       <c r="E198" t="n">
-        <v>0.05820044736870371</v>
+        <v>3.33464</v>
       </c>
       <c r="F198" t="n">
         <v>0.394992</v>
@@ -5979,7 +5979,7 @@
         <v>1.412331405867617</v>
       </c>
       <c r="E199" t="n">
-        <v>0.08067644841003628</v>
+        <v>4.62242</v>
       </c>
       <c r="F199" t="n">
         <v>-0.131486</v>
@@ -6007,7 +6007,7 @@
         <v>1.398670797578901</v>
       </c>
       <c r="E200" t="n">
-        <v>0.08902557995280157</v>
+        <v>5.10079</v>
       </c>
       <c r="F200" t="n">
         <v>-0.371466</v>
@@ -6035,7 +6035,7 @@
         <v>1.426993342661415</v>
       </c>
       <c r="E201" t="n">
-        <v>0.0974506333180286</v>
+        <v>5.58351</v>
       </c>
       <c r="F201" t="n">
         <v>-0.158364</v>
@@ -6063,7 +6063,7 @@
         <v>1.416940365717626</v>
       </c>
       <c r="E202" t="n">
-        <v>0.1001794556035217</v>
+        <v>5.73986</v>
       </c>
       <c r="F202" t="n">
         <v>-0.0250728</v>
@@ -6091,7 +6091,7 @@
         <v>1.376470123177397</v>
       </c>
       <c r="E203" t="n">
-        <v>0.1027185605993231</v>
+        <v>5.88534</v>
       </c>
       <c r="F203" t="n">
         <v>-0.39792</v>
@@ -6119,7 +6119,7 @@
         <v>1.445046712047745</v>
       </c>
       <c r="E204" t="n">
-        <v>0.001678411583143615</v>
+        <v>0.0961659</v>
       </c>
       <c r="F204" t="n">
         <v>0.0346211</v>
@@ -6147,7 +6147,7 @@
         <v>1.452339491992144</v>
       </c>
       <c r="E205" t="n">
-        <v>0.005067057337682457</v>
+        <v>0.290321</v>
       </c>
       <c r="F205" t="n">
         <v>0.138849</v>
@@ -6175,7 +6175,7 @@
         <v>1.477829489487877</v>
       </c>
       <c r="E206" t="n">
-        <v>0.008080123945155388</v>
+        <v>0.462957</v>
       </c>
       <c r="F206" t="n">
         <v>0.0495043</v>
@@ -6203,7 +6203,7 @@
         <v>1.50248793672362</v>
       </c>
       <c r="E207" t="n">
-        <v>0.01133432524208386</v>
+        <v>0.649409</v>
       </c>
       <c r="F207" t="n">
         <v>0.110256</v>
@@ -6231,7 +6231,7 @@
         <v>1.451588784745873</v>
       </c>
       <c r="E208" t="n">
-        <v>0.01902967390034457</v>
+        <v>1.09032</v>
       </c>
       <c r="F208" t="n">
         <v>0.0711478</v>
@@ -6259,7 +6259,7 @@
         <v>1.461642911247477</v>
       </c>
       <c r="E209" t="n">
-        <v>0.0342571480252195</v>
+        <v>1.96279</v>
       </c>
       <c r="F209" t="n">
         <v>0.100978</v>
@@ -6287,7 +6287,7 @@
         <v>1.45547243189282</v>
       </c>
       <c r="E210" t="n">
-        <v>0.04089149357790035</v>
+        <v>2.34291</v>
       </c>
       <c r="F210" t="n">
         <v>0.141417</v>
@@ -6315,7 +6315,7 @@
         <v>1.455942993389508</v>
       </c>
       <c r="E211" t="n">
-        <v>0.04605522470285077</v>
+        <v>2.63877</v>
       </c>
       <c r="F211" t="n">
         <v>-0.0384936</v>
@@ -6343,7 +6343,7 @@
         <v>1.44705908656143</v>
       </c>
       <c r="E212" t="n">
-        <v>0.05042500555106897</v>
+        <v>2.88914</v>
       </c>
       <c r="F212" t="n">
         <v>0.168335</v>
@@ -6371,7 +6371,7 @@
         <v>1.448568258660944</v>
       </c>
       <c r="E213" t="n">
-        <v>0.0559580483457414</v>
+        <v>3.20616</v>
       </c>
       <c r="F213" t="n">
         <v>0.148223</v>
@@ -6399,7 +6399,7 @@
         <v>1.448012430885868</v>
       </c>
       <c r="E214" t="n">
-        <v>0.06217019875236481</v>
+        <v>3.56209</v>
       </c>
       <c r="F214" t="n">
         <v>-0.0171806</v>
@@ -6427,7 +6427,7 @@
         <v>1.470221071811991</v>
       </c>
       <c r="E215" t="n">
-        <v>0.07018562334214878</v>
+        <v>4.02134</v>
       </c>
       <c r="F215" t="n">
         <v>-0.385581</v>
@@ -6455,7 +6455,7 @@
         <v>1.470897685088939</v>
       </c>
       <c r="E216" t="n">
-        <v>0.0803959739992408</v>
+        <v>4.60635</v>
       </c>
       <c r="F216" t="n">
         <v>-0.209154</v>
@@ -6483,7 +6483,7 @@
         <v>1.459198410086853</v>
       </c>
       <c r="E217" t="n">
-        <v>0.08620355708525193</v>
+        <v>4.9391</v>
       </c>
       <c r="F217" t="n">
         <v>-0.379335</v>
@@ -6511,7 +6511,7 @@
         <v>1.437967315344824</v>
       </c>
       <c r="E218" t="n">
-        <v>0.09100530692333873</v>
+        <v>5.21422</v>
       </c>
       <c r="F218" t="n">
         <v>-0.159063</v>
@@ -6539,7 +6539,7 @@
         <v>1.444925603621169</v>
       </c>
       <c r="E219" t="n">
-        <v>0.09530806712828035</v>
+        <v>5.46075</v>
       </c>
       <c r="F219" t="n">
         <v>-0.223016</v>
@@ -6567,7 +6567,7 @@
         <v>1.496165097841812</v>
       </c>
       <c r="E220" t="n">
-        <v>0.09965323883404544</v>
+        <v>5.70971</v>
       </c>
       <c r="F220" t="n">
         <v>-0.150313</v>
@@ -6595,7 +6595,7 @@
         <v>1.462210655138308</v>
       </c>
       <c r="E221" t="n">
-        <v>0.1025986564797111</v>
+        <v>5.87847</v>
       </c>
       <c r="F221" t="n">
         <v>-0.0161398</v>
@@ -6623,7 +6623,7 @@
         <v>1.452959049663823</v>
       </c>
       <c r="E222" t="n">
-        <v>0.1065572377561594</v>
+        <v>6.10528</v>
       </c>
       <c r="F222" t="n">
         <v>-0.0622883</v>
@@ -6651,7 +6651,7 @@
         <v>1.48205937802775</v>
       </c>
       <c r="E223" t="n">
-        <v>0.00258238916125081</v>
+        <v>0.14796</v>
       </c>
       <c r="F223" t="n">
         <v>-0.20753</v>
@@ -6679,7 +6679,7 @@
         <v>1.471281754117817</v>
       </c>
       <c r="E224" t="n">
-        <v>0.04005303740524227</v>
+        <v>2.29487</v>
       </c>
       <c r="F224" t="n">
         <v>0.0774096</v>
@@ -6707,7 +6707,7 @@
         <v>1.479986486424792</v>
       </c>
       <c r="E225" t="n">
-        <v>0.04756563263752666</v>
+        <v>2.72531</v>
       </c>
       <c r="F225" t="n">
         <v>-0.0693385</v>
@@ -6735,7 +6735,7 @@
         <v>1.465366848267013</v>
       </c>
       <c r="E226" t="n">
-        <v>0.0593110003717477</v>
+        <v>3.39827</v>
       </c>
       <c r="F226" t="n">
         <v>0.135925</v>
@@ -6763,7 +6763,7 @@
         <v>1.470649516370233</v>
       </c>
       <c r="E227" t="n">
-        <v>0.1071993443879681</v>
+        <v>6.14207</v>
       </c>
       <c r="F227" t="n">
         <v>-0.281703</v>
@@ -6791,7 +6791,7 @@
         <v>1.412550884039226</v>
       </c>
       <c r="E228" t="n">
-        <v>0.003006294729975193</v>
+        <v>0.172248</v>
       </c>
       <c r="F228" t="n">
         <v>-0.08005909999999999</v>
@@ -6819,7 +6819,7 @@
         <v>1.420179566111272</v>
       </c>
       <c r="E229" t="n">
-        <v>0.007256695057356983</v>
+        <v>0.415778</v>
       </c>
       <c r="F229" t="n">
         <v>0.0589381</v>
@@ -6847,7 +6847,7 @@
         <v>1.426236305806299</v>
       </c>
       <c r="E230" t="n">
-        <v>0.01090354307610662</v>
+        <v>0.624727</v>
       </c>
       <c r="F230" t="n">
         <v>0.148787</v>
@@ -6875,7 +6875,7 @@
         <v>1.42724559904734</v>
       </c>
       <c r="E231" t="n">
-        <v>0.08099689086070246</v>
+        <v>4.64078</v>
       </c>
       <c r="F231" t="n">
         <v>-0.207461</v>
@@ -6903,7 +6903,7 @@
         <v>1.425759446751099</v>
       </c>
       <c r="E232" t="n">
-        <v>0.1006199767067251</v>
+        <v>5.7651</v>
       </c>
       <c r="F232" t="n">
         <v>-0.0628537</v>
@@ -6931,7 +6931,7 @@
         <v>1.407895592719858</v>
       </c>
       <c r="E233" t="n">
-        <v>0.1033386760825567</v>
+        <v>5.92087</v>
       </c>
       <c r="F233" t="n">
         <v>-0.110957</v>
@@ -6959,7 +6959,7 @@
         <v>1.409421867291692</v>
       </c>
       <c r="E234" t="n">
-        <v>0.1072958610956034</v>
+        <v>6.1476</v>
       </c>
       <c r="F234" t="n">
         <v>0.0130041</v>
@@ -6987,7 +6987,7 @@
         <v>1.448078036571234</v>
       </c>
       <c r="E235" t="n">
-        <v>0.003417895727473016</v>
+        <v>0.195831</v>
       </c>
       <c r="F235" t="n">
         <v>-0.0278717</v>
@@ -7015,7 +7015,7 @@
         <v>1.475527024489894</v>
       </c>
       <c r="E236" t="n">
-        <v>0.006761684774906351</v>
+        <v>0.387416</v>
       </c>
       <c r="F236" t="n">
         <v>0.0187117</v>
@@ -7043,7 +7043,7 @@
         <v>1.456866500404207</v>
       </c>
       <c r="E237" t="n">
-        <v>0.01399422447541573</v>
+        <v>0.80181</v>
       </c>
       <c r="F237" t="n">
         <v>0.128113</v>
@@ -7071,7 +7071,7 @@
         <v>1.466553783534719</v>
       </c>
       <c r="E238" t="n">
-        <v>0.02032069394804478</v>
+        <v>1.16429</v>
       </c>
       <c r="F238" t="n">
         <v>0.11686</v>
@@ -7099,7 +7099,7 @@
         <v>1.444025623041364</v>
       </c>
       <c r="E239" t="n">
-        <v>0.04544767559023154</v>
+        <v>2.60396</v>
       </c>
       <c r="F239" t="n">
         <v>0.0650039</v>
@@ -7127,7 +7127,7 @@
         <v>1.445268141211173</v>
       </c>
       <c r="E240" t="n">
-        <v>0.05569153656896186</v>
+        <v>3.19089</v>
       </c>
       <c r="F240" t="n">
         <v>0.0574452</v>
@@ -7155,7 +7155,7 @@
         <v>1.446060164723446</v>
       </c>
       <c r="E241" t="n">
-        <v>0.07984549715316179</v>
+        <v>4.57481</v>
       </c>
       <c r="F241" t="n">
         <v>-0.0104943</v>
@@ -7183,7 +7183,7 @@
         <v>1.445416894878429</v>
       </c>
       <c r="E242" t="n">
-        <v>0.0868891224154353</v>
+        <v>4.97838</v>
       </c>
       <c r="F242" t="n">
         <v>0.0360523</v>
@@ -7211,7 +7211,7 @@
         <v>1.467242311276498</v>
       </c>
       <c r="E243" t="n">
-        <v>0.09793147152695303</v>
+        <v>5.61106</v>
       </c>
       <c r="F243" t="n">
         <v>0.0759827</v>
@@ -7239,7 +7239,7 @@
         <v>1.465185995019062</v>
       </c>
       <c r="E244" t="n">
-        <v>0.1036308441993405</v>
+        <v>5.93761</v>
       </c>
       <c r="F244" t="n">
         <v>-0.0183127</v>
@@ -7267,7 +7267,7 @@
         <v>1.450978979861528</v>
       </c>
       <c r="E245" t="n">
-        <v>0.1068679063630144</v>
+        <v>6.12308</v>
       </c>
       <c r="F245" t="n">
         <v>0.0083249</v>
@@ -7295,7 +7295,7 @@
         <v>1.638654936220558</v>
       </c>
       <c r="E246" t="n">
-        <v>0.001636124000697045</v>
+        <v>0.09374300000000001</v>
       </c>
       <c r="F246" t="n">
         <v>0.0116763</v>
@@ -7323,7 +7323,7 @@
         <v>1.636917835445628</v>
       </c>
       <c r="E247" t="n">
-        <v>0.004946908871975168</v>
+        <v>0.283437</v>
       </c>
       <c r="F247" t="n">
         <v>0.0143155</v>
@@ -7351,7 +7351,7 @@
         <v>1.630883196308062</v>
       </c>
       <c r="E248" t="n">
-        <v>0.008057556837927101</v>
+        <v>0.461664</v>
       </c>
       <c r="F248" t="n">
         <v>0.0840181</v>
@@ -7379,7 +7379,7 @@
         <v>1.624567634787792</v>
       </c>
       <c r="E249" t="n">
-        <v>0.01117345824492754</v>
+        <v>0.640192</v>
       </c>
       <c r="F249" t="n">
         <v>0.0433752</v>
@@ -7407,7 +7407,7 @@
         <v>1.590958830391283</v>
       </c>
       <c r="E250" t="n">
-        <v>0.01749186429641237</v>
+        <v>1.00221</v>
       </c>
       <c r="F250" t="n">
         <v>0.07867830000000001</v>
@@ -7435,7 +7435,7 @@
         <v>1.611638917375725</v>
       </c>
       <c r="E251" t="n">
-        <v>0.02856667653201719</v>
+        <v>1.63675</v>
       </c>
       <c r="F251" t="n">
         <v>0.253842</v>
@@ -7463,7 +7463,7 @@
         <v>1.620737486454855</v>
       </c>
       <c r="E252" t="n">
-        <v>0.03885050555061818</v>
+        <v>2.22597</v>
       </c>
       <c r="F252" t="n">
         <v>0.32266</v>
@@ -7491,7 +7491,7 @@
         <v>1.624361412986654</v>
       </c>
       <c r="E253" t="n">
-        <v>0.04787525404683046</v>
+        <v>2.74305</v>
       </c>
       <c r="F253" t="n">
         <v>-0.0113255</v>
@@ -7519,7 +7519,7 @@
         <v>1.615821772349909</v>
       </c>
       <c r="E254" t="n">
-        <v>0.05788855703137232</v>
+        <v>3.31677</v>
       </c>
       <c r="F254" t="n">
         <v>-0.115091</v>
@@ -7547,7 +7547,7 @@
         <v>1.626111927267001</v>
       </c>
       <c r="E255" t="n">
-        <v>0.09839869616771191</v>
+        <v>5.63783</v>
       </c>
       <c r="F255" t="n">
         <v>-0.140645</v>
@@ -7575,7 +7575,7 @@
         <v>1.629984662504528</v>
       </c>
       <c r="E256" t="n">
-        <v>0.1015181231398014</v>
+        <v>5.81656</v>
       </c>
       <c r="F256" t="n">
         <v>-0.059704</v>
@@ -7603,7 +7603,7 @@
         <v>1.639109514340027</v>
       </c>
       <c r="E257" t="n">
-        <v>0.104714693664829</v>
+        <v>5.99971</v>
       </c>
       <c r="F257" t="n">
         <v>-0.149684</v>
@@ -7631,7 +7631,7 @@
         <v>1.638020146396252</v>
       </c>
       <c r="E258" t="n">
-        <v>0.1080152858132755</v>
+        <v>6.18882</v>
       </c>
       <c r="F258" t="n">
         <v>-0.0756371</v>
@@ -7659,7 +7659,7 @@
         <v>1.687089209259546</v>
       </c>
       <c r="E259" t="n">
-        <v>0.001756202653234254</v>
+        <v>0.100623</v>
       </c>
       <c r="F259" t="n">
         <v>0.0281924</v>
@@ -7687,7 +7687,7 @@
         <v>1.67251307917158</v>
       </c>
       <c r="E260" t="n">
-        <v>0.00497413600830628</v>
+        <v>0.284997</v>
       </c>
       <c r="F260" t="n">
         <v>0.0725075</v>
@@ -7715,7 +7715,7 @@
         <v>1.663361055213209</v>
       </c>
       <c r="E261" t="n">
-        <v>0.008305201605492578</v>
+        <v>0.475853</v>
       </c>
       <c r="F261" t="n">
         <v>0.208214</v>
@@ -7743,7 +7743,7 @@
         <v>1.667324203626877</v>
       </c>
       <c r="E262" t="n">
-        <v>0.01146384612587436</v>
+        <v>0.65683</v>
       </c>
       <c r="F262" t="n">
         <v>0.273676</v>
@@ -7771,7 +7771,7 @@
         <v>1.664487909238154</v>
       </c>
       <c r="E263" t="n">
-        <v>0.01474267401854846</v>
+        <v>0.844693</v>
       </c>
       <c r="F263" t="n">
         <v>0.247133</v>
@@ -7799,7 +7799,7 @@
         <v>1.66290408622987</v>
       </c>
       <c r="E264" t="n">
-        <v>0.01808562530794084</v>
+        <v>1.03623</v>
       </c>
       <c r="F264" t="n">
         <v>0.257047</v>
@@ -7827,7 +7827,7 @@
         <v>1.673615846005289</v>
       </c>
       <c r="E265" t="n">
-        <v>0.0213916279770685</v>
+        <v>1.22565</v>
       </c>
       <c r="F265" t="n">
         <v>0.249813</v>
@@ -7855,7 +7855,7 @@
         <v>1.668229600504679</v>
       </c>
       <c r="E266" t="n">
-        <v>0.024560098701139</v>
+        <v>1.40719</v>
       </c>
       <c r="F266" t="n">
         <v>0.456992</v>
@@ -7883,7 +7883,7 @@
         <v>1.668112706024386</v>
       </c>
       <c r="E267" t="n">
-        <v>0.02945278019325471</v>
+        <v>1.68752</v>
       </c>
       <c r="F267" t="n">
         <v>0.498534</v>
@@ -7911,7 +7911,7 @@
         <v>1.675210434542479</v>
       </c>
       <c r="E268" t="n">
-        <v>0.03685454701803747</v>
+        <v>2.11161</v>
       </c>
       <c r="F268" t="n">
         <v>0.342191</v>
@@ -7939,7 +7939,7 @@
         <v>1.683597339033297</v>
       </c>
       <c r="E269" t="n">
-        <v>0.04662908896090651</v>
+        <v>2.67165</v>
       </c>
       <c r="F269" t="n">
         <v>0.0419558</v>
@@ -7967,7 +7967,7 @@
         <v>1.675720740457669</v>
       </c>
       <c r="E270" t="n">
-        <v>0.0565113177186236</v>
+        <v>3.23786</v>
       </c>
       <c r="F270" t="n">
         <v>-0.151178</v>
@@ -7995,7 +7995,7 @@
         <v>1.669616722484535</v>
       </c>
       <c r="E271" t="n">
-        <v>0.06780394704487731</v>
+        <v>3.88488</v>
       </c>
       <c r="F271" t="n">
         <v>-0.113908</v>
@@ -8023,7 +8023,7 @@
         <v>1.661508350866766</v>
       </c>
       <c r="E272" t="n">
-        <v>0.08035722768984652</v>
+        <v>4.60413</v>
       </c>
       <c r="F272" t="n">
         <v>-0.580404</v>
@@ -8051,7 +8051,7 @@
         <v>1.663391114560854</v>
       </c>
       <c r="E273" t="n">
-        <v>0.08961672297045205</v>
+        <v>5.13466</v>
       </c>
       <c r="F273" t="n">
         <v>-0.373527</v>
@@ -8079,7 +8079,7 @@
         <v>1.663953124339745</v>
       </c>
       <c r="E274" t="n">
-        <v>0.09768433290487062</v>
+        <v>5.5969</v>
       </c>
       <c r="F274" t="n">
         <v>-0.360416</v>
@@ -8107,7 +8107,7 @@
         <v>1.676773687770654</v>
       </c>
       <c r="E275" t="n">
-        <v>0.1014833910876867</v>
+        <v>5.81457</v>
       </c>
       <c r="F275" t="n">
         <v>-0.364693</v>
@@ -8135,7 +8135,7 @@
         <v>1.676892960209446</v>
       </c>
       <c r="E276" t="n">
-        <v>0.1047433170645617</v>
+        <v>6.00135</v>
       </c>
       <c r="F276" t="n">
         <v>-0.114714</v>
@@ -8163,7 +8163,7 @@
         <v>1.690931695841083</v>
       </c>
       <c r="E277" t="n">
-        <v>0.1079880586769444</v>
+        <v>6.18726</v>
       </c>
       <c r="F277" t="n">
         <v>-0.255481</v>
@@ -8191,7 +8191,7 @@
         <v>1.683226069189757</v>
       </c>
       <c r="E278" t="n">
-        <v>0.001720702656248689</v>
+        <v>0.098589</v>
       </c>
       <c r="F278" t="n">
         <v>0.131694</v>
@@ -8219,7 +8219,7 @@
         <v>1.688907931179198</v>
       </c>
       <c r="E279" t="n">
-        <v>0.005554108918743994</v>
+        <v>0.318227</v>
       </c>
       <c r="F279" t="n">
         <v>0.0884076</v>
@@ -8247,7 +8247,7 @@
         <v>1.691883565733765</v>
       </c>
       <c r="E280" t="n">
-        <v>0.009086096819419881</v>
+        <v>0.520595</v>
       </c>
       <c r="F280" t="n">
         <v>0.0388802</v>
@@ -8275,7 +8275,7 @@
         <v>1.673579995100324</v>
       </c>
       <c r="E281" t="n">
-        <v>0.01413088375584689</v>
+        <v>0.80964</v>
       </c>
       <c r="F281" t="n">
         <v>0.207393</v>
@@ -8303,7 +8303,7 @@
         <v>1.693496383226135</v>
       </c>
       <c r="E282" t="n">
-        <v>0.02197125182165582</v>
+        <v>1.25886</v>
       </c>
       <c r="F282" t="n">
         <v>0.0553246</v>
@@ -8331,7 +8331,7 @@
         <v>1.690331328467884</v>
       </c>
       <c r="E283" t="n">
-        <v>0.03233117719564376</v>
+        <v>1.85244</v>
       </c>
       <c r="F283" t="n">
         <v>0.555882</v>
@@ -8359,7 +8359,7 @@
         <v>1.693496383226135</v>
       </c>
       <c r="E284" t="n">
-        <v>0.06698521309276677</v>
+        <v>3.83797</v>
       </c>
       <c r="F284" t="n">
         <v>-0.108496</v>
@@ -8387,7 +8387,7 @@
         <v>1.704303376749574</v>
       </c>
       <c r="E285" t="n">
-        <v>0.07698507704206828</v>
+        <v>4.41092</v>
       </c>
       <c r="F285" t="n">
         <v>0.0335076</v>
@@ -8415,7 +8415,7 @@
         <v>1.674825364030531</v>
       </c>
       <c r="E286" t="n">
-        <v>0.08817490647537954</v>
+        <v>5.05205</v>
       </c>
       <c r="F286" t="n">
         <v>-0.226327</v>
@@ -8443,7 +8443,7 @@
         <v>1.673158689425483</v>
       </c>
       <c r="E287" t="n">
-        <v>0.09648756063677813</v>
+        <v>5.52833</v>
       </c>
       <c r="F287" t="n">
         <v>0.0849847</v>
@@ -8471,7 +8471,7 @@
         <v>1.67606085808362</v>
       </c>
       <c r="E288" t="n">
-        <v>0.1027780763268161</v>
+        <v>5.88875</v>
       </c>
       <c r="F288" t="n">
         <v>-0.135714</v>
@@ -8499,7 +8499,7 @@
         <v>1.678007747300351</v>
       </c>
       <c r="E289" t="n">
-        <v>0.1075030316778151</v>
+        <v>6.15947</v>
       </c>
       <c r="F289" t="n">
         <v>0.0439917</v>
@@ -8527,7 +8527,7 @@
         <v>1.624444520443835</v>
       </c>
       <c r="E290" t="n">
-        <v>0.001665915025699336</v>
+        <v>0.0954499</v>
       </c>
       <c r="F290" t="n">
         <v>0.14309</v>
@@ -8555,7 +8555,7 @@
         <v>1.634649809592256</v>
       </c>
       <c r="E291" t="n">
-        <v>0.005053234330006662</v>
+        <v>0.289529</v>
       </c>
       <c r="F291" t="n">
         <v>0.0951029</v>
@@ -8583,7 +8583,7 @@
         <v>1.642796396392444</v>
       </c>
       <c r="E292" t="n">
-        <v>0.008235475701875404</v>
+        <v>0.471858</v>
       </c>
       <c r="F292" t="n">
         <v>0.139608</v>
@@ -8611,7 +8611,7 @@
         <v>1.635487694848237</v>
       </c>
       <c r="E293" t="n">
-        <v>0.01118548356347378</v>
+        <v>0.640881</v>
       </c>
       <c r="F293" t="n">
         <v>0.153944</v>
@@ -8639,7 +8639,7 @@
         <v>1.615103711840203</v>
       </c>
       <c r="E294" t="n">
-        <v>0.01485627749956077</v>
+        <v>0.851202</v>
       </c>
       <c r="F294" t="n">
         <v>0.311101</v>
@@ -8667,7 +8667,7 @@
         <v>1.629156223325437</v>
       </c>
       <c r="E295" t="n">
-        <v>0.03042510311954075</v>
+        <v>1.74323</v>
       </c>
       <c r="F295" t="n">
         <v>0.265784</v>
@@ -8695,7 +8695,7 @@
         <v>1.627866702159609</v>
       </c>
       <c r="E296" t="n">
-        <v>0.03917897651584351</v>
+        <v>2.24479</v>
       </c>
       <c r="F296" t="n">
         <v>0.335962</v>
@@ -8723,7 +8723,7 @@
         <v>1.619070721123694</v>
       </c>
       <c r="E297" t="n">
-        <v>0.04535255514599786</v>
+        <v>2.59851</v>
       </c>
       <c r="F297" t="n">
         <v>-0.033104</v>
@@ -8751,7 +8751,7 @@
         <v>1.618125458671237</v>
       </c>
       <c r="E298" t="n">
-        <v>0.05127567902849101</v>
+        <v>2.93788</v>
       </c>
       <c r="F298" t="n">
         <v>0.0856304</v>
@@ -8779,7 +8779,7 @@
         <v>1.617096162879623</v>
       </c>
       <c r="E299" t="n">
-        <v>0.06030461631490808</v>
+        <v>3.4552</v>
       </c>
       <c r="F299" t="n">
         <v>0.0240557</v>
@@ -8807,7 +8807,7 @@
         <v>1.648681291214284</v>
       </c>
       <c r="E300" t="n">
-        <v>0.07039663364871489</v>
+        <v>4.03343</v>
       </c>
       <c r="F300" t="n">
         <v>-0.444091</v>
@@ -8835,7 +8835,7 @@
         <v>1.630441657956518</v>
       </c>
       <c r="E301" t="n">
-        <v>0.08190812726316869</v>
+        <v>4.69299</v>
       </c>
       <c r="F301" t="n">
         <v>-0.12967</v>
@@ -8863,7 +8863,7 @@
         <v>1.621949444341592</v>
       </c>
       <c r="E302" t="n">
-        <v>0.09577825882876762</v>
+        <v>5.48769</v>
       </c>
       <c r="F302" t="n">
         <v>-0.318817</v>
@@ -8891,7 +8891,7 @@
         <v>1.636789540533541</v>
       </c>
       <c r="E303" t="n">
-        <v>0.09942913855808935</v>
+        <v>5.69687</v>
       </c>
       <c r="F303" t="n">
         <v>-0.0442793</v>
@@ -8919,7 +8919,7 @@
         <v>1.638810544266786</v>
       </c>
       <c r="E304" t="n">
-        <v>0.1024414023141064</v>
+        <v>5.86946</v>
       </c>
       <c r="F304" t="n">
         <v>-0.10433</v>
@@ -8947,7 +8947,7 @@
         <v>1.631263314121911</v>
       </c>
       <c r="E305" t="n">
-        <v>0.106698609425571</v>
+        <v>6.11338</v>
       </c>
       <c r="F305" t="n">
         <v>-0.0468691</v>
@@ -8975,7 +8975,7 @@
         <v>1.709286400811754</v>
       </c>
       <c r="E306" t="n">
-        <v>0.001588829068626502</v>
+        <v>0.09103319999999999</v>
       </c>
       <c r="F306" t="n">
         <v>0.0785074</v>
@@ -9003,7 +9003,7 @@
         <v>1.708095430589287</v>
       </c>
       <c r="E307" t="n">
-        <v>0.004942458282382582</v>
+        <v>0.283182</v>
       </c>
       <c r="F307" t="n">
         <v>0.0920092</v>
@@ -9031,7 +9031,7 @@
         <v>1.710301143073932</v>
       </c>
       <c r="E308" t="n">
-        <v>0.008189852795228271</v>
+        <v>0.469244</v>
       </c>
       <c r="F308" t="n">
         <v>0.237835</v>
@@ -9059,7 +9059,7 @@
         <v>1.685229954635272</v>
       </c>
       <c r="E309" t="n">
-        <v>0.01125952043034338</v>
+        <v>0.645123</v>
       </c>
       <c r="F309" t="n">
         <v>0.179849</v>
@@ -9087,7 +9087,7 @@
         <v>1.67681245224384</v>
       </c>
       <c r="E310" t="n">
-        <v>0.01573009404286425</v>
+        <v>0.901268</v>
       </c>
       <c r="F310" t="n">
         <v>0.405792</v>
@@ -9115,7 +9115,7 @@
         <v>1.679949404000013</v>
       </c>
       <c r="E311" t="n">
-        <v>0.02202849862112123</v>
+        <v>1.26214</v>
       </c>
       <c r="F311" t="n">
         <v>0.427738</v>
@@ -9143,7 +9143,7 @@
         <v>1.685045993437568</v>
       </c>
       <c r="E312" t="n">
-        <v>0.02730707241085288</v>
+        <v>1.56458</v>
       </c>
       <c r="F312" t="n">
         <v>0.336794</v>
@@ -9171,7 +9171,7 @@
         <v>1.677349099025006</v>
       </c>
       <c r="E313" t="n">
-        <v>0.0317335764597609</v>
+        <v>1.8182</v>
       </c>
       <c r="F313" t="n">
         <v>0.34717</v>
@@ -9199,7 +9199,7 @@
         <v>1.687029934529912</v>
       </c>
       <c r="E314" t="n">
-        <v>0.03605413902307286</v>
+        <v>2.06575</v>
       </c>
       <c r="F314" t="n">
         <v>0.155353</v>
@@ -9227,7 +9227,7 @@
         <v>1.67310489808619</v>
       </c>
       <c r="E315" t="n">
-        <v>0.0413658740685924</v>
+        <v>2.37009</v>
       </c>
       <c r="F315" t="n">
         <v>0.243799</v>
@@ -9255,7 +9255,7 @@
         <v>1.686048635122961</v>
       </c>
       <c r="E316" t="n">
-        <v>0.04552656447242169</v>
+        <v>2.60848</v>
       </c>
       <c r="F316" t="n">
         <v>-0.0841826</v>
@@ -9283,7 +9283,7 @@
         <v>1.682625923965276</v>
       </c>
       <c r="E317" t="n">
-        <v>0.04934359954653329</v>
+        <v>2.82718</v>
       </c>
       <c r="F317" t="n">
         <v>0.0410112</v>
@@ -9311,7 +9311,7 @@
         <v>1.669514899604074</v>
       </c>
       <c r="E318" t="n">
-        <v>0.05383834596919428</v>
+        <v>3.08471</v>
       </c>
       <c r="F318" t="n">
         <v>0.107844</v>
@@ -9339,7 +9339,7 @@
         <v>1.679797606856255</v>
       </c>
       <c r="E319" t="n">
-        <v>0.05790932644947105</v>
+        <v>3.31796</v>
       </c>
       <c r="F319" t="n">
         <v>-0.0159166</v>
@@ -9367,7 +9367,7 @@
         <v>1.667845916144534</v>
       </c>
       <c r="E320" t="n">
-        <v>0.06469342125197301</v>
+        <v>3.70666</v>
       </c>
       <c r="F320" t="n">
         <v>-0.09146310000000001</v>
@@ -9395,7 +9395,7 @@
         <v>1.674389440960495</v>
       </c>
       <c r="E321" t="n">
-        <v>0.0732268595637489</v>
+        <v>4.19559</v>
       </c>
       <c r="F321" t="n">
         <v>-0.06871620000000001</v>
@@ -9423,7 +9423,7 @@
         <v>1.700544030597267</v>
       </c>
       <c r="E322" t="n">
-        <v>0.08394195944051767</v>
+        <v>4.80952</v>
       </c>
       <c r="F322" t="n">
         <v>-0.29739</v>
@@ -9451,7 +9451,7 @@
         <v>1.740723987311027</v>
       </c>
       <c r="E323" t="n">
-        <v>0.09743457628891024</v>
+        <v>5.58259</v>
       </c>
       <c r="F323" t="n">
         <v>-0.170878</v>
@@ -9479,7 +9479,7 @@
         <v>1.736162434796929</v>
       </c>
       <c r="E324" t="n">
-        <v>0.1026105247186246</v>
+        <v>5.87915</v>
       </c>
       <c r="F324" t="n">
         <v>-0.0327145</v>
@@ -9507,7 +9507,7 @@
         <v>1.714523257351734</v>
       </c>
       <c r="E325" t="n">
-        <v>0.1070803129329821</v>
+        <v>6.13525</v>
       </c>
       <c r="F325" t="n">
         <v>0.00587702</v>
@@ -9535,7 +9535,7 @@
         <v>1.691957446273398</v>
       </c>
       <c r="E326" t="n">
-        <v>0.002178240719659003</v>
+        <v>0.124804</v>
       </c>
       <c r="F326" t="n">
         <v>-0.10564</v>
@@ -9563,7 +9563,7 @@
         <v>1.694426156549762</v>
       </c>
       <c r="E327" t="n">
-        <v>0.007853876914219363</v>
+        <v>0.449994</v>
       </c>
       <c r="F327" t="n">
         <v>0.336631</v>
@@ -9591,7 +9591,7 @@
         <v>1.692713797427078</v>
       </c>
       <c r="E328" t="n">
-        <v>0.014539238440936</v>
+        <v>0.833037</v>
       </c>
       <c r="F328" t="n">
         <v>0.219809</v>
@@ -9619,7 +9619,7 @@
         <v>1.70651106061461</v>
       </c>
       <c r="E329" t="n">
-        <v>0.02436409822614004</v>
+        <v>1.39596</v>
       </c>
       <c r="F329" t="n">
         <v>0.129282</v>
@@ -9647,7 +9647,7 @@
         <v>1.6822782171805</v>
       </c>
       <c r="E330" t="n">
-        <v>0.03452243807152264</v>
+        <v>1.97799</v>
       </c>
       <c r="F330" t="n">
         <v>0.177901</v>
@@ -9675,7 +9675,7 @@
         <v>1.694668109099832</v>
       </c>
       <c r="E331" t="n">
-        <v>0.04407095987625842</v>
+        <v>2.52508</v>
       </c>
       <c r="F331" t="n">
         <v>-0.0185757</v>
@@ -9703,7 +9703,7 @@
         <v>1.666037214470313</v>
       </c>
       <c r="E332" t="n">
-        <v>0.06851289978703741</v>
+        <v>3.9255</v>
       </c>
       <c r="F332" t="n">
         <v>-0.316461</v>
@@ -9731,7 +9731,7 @@
         <v>1.674449163157843</v>
       </c>
       <c r="E333" t="n">
-        <v>0.09062203261960078</v>
+        <v>5.19226</v>
       </c>
       <c r="F333" t="n">
         <v>-0.241717</v>
@@ -9759,7 +9759,7 @@
         <v>1.691862878604528</v>
       </c>
       <c r="E334" t="n">
-        <v>0.1004337500755373</v>
+        <v>5.75443</v>
       </c>
       <c r="F334" t="n">
         <v>-0.139862</v>
@@ -9787,7 +9787,7 @@
         <v>1.68962125933595</v>
       </c>
       <c r="E335" t="n">
-        <v>0.1071487298396603</v>
+        <v>6.13917</v>
       </c>
       <c r="F335" t="n">
         <v>-0.159634</v>
@@ -9815,7 +9815,7 @@
         <v>1.591103390732356</v>
       </c>
       <c r="E336" t="n">
-        <v>0.004545099171581034</v>
+        <v>0.260415</v>
       </c>
       <c r="F336" t="n">
         <v>0.15354</v>
@@ -9843,7 +9843,7 @@
         <v>1.630714567298643</v>
       </c>
       <c r="E337" t="n">
-        <v>0.008449522881339988</v>
+        <v>0.484122</v>
       </c>
       <c r="F337" t="n">
         <v>0.157046</v>
@@ -9871,7 +9871,7 @@
         <v>1.63629459450308</v>
       </c>
       <c r="E338" t="n">
-        <v>0.01110601872263048</v>
+        <v>0.636328</v>
       </c>
       <c r="F338" t="n">
         <v>0.0708785</v>
@@ -9899,7 +9899,7 @@
         <v>1.62565986602364</v>
       </c>
       <c r="E339" t="n">
-        <v>0.04088660665599476</v>
+        <v>2.34263</v>
       </c>
       <c r="F339" t="n">
         <v>0.231829</v>
@@ -9927,7 +9927,7 @@
         <v>1.615827961139428</v>
       </c>
       <c r="E340" t="n">
-        <v>0.05058592490810285</v>
+        <v>2.89836</v>
       </c>
       <c r="F340" t="n">
         <v>0.0930666</v>
@@ -9955,7 +9955,7 @@
         <v>1.628376492092661</v>
       </c>
       <c r="E341" t="n">
-        <v>0.06160977352954944</v>
+        <v>3.52998</v>
       </c>
       <c r="F341" t="n">
         <v>-0.0268148</v>
@@ -9983,7 +9983,7 @@
         <v>1.628050982002714</v>
       </c>
       <c r="E342" t="n">
-        <v>0.07507917749889048</v>
+        <v>4.30172</v>
       </c>
       <c r="F342" t="n">
         <v>-0.241036</v>
@@ -10011,7 +10011,7 @@
         <v>1.626520826795649</v>
       </c>
       <c r="E343" t="n">
-        <v>0.08296422599355045</v>
+        <v>4.7535</v>
       </c>
       <c r="F343" t="n">
         <v>-0.125454</v>
@@ -10039,7 +10039,7 @@
         <v>1.622078913000228</v>
       </c>
       <c r="E344" t="n">
-        <v>0.09490995752590045</v>
+        <v>5.43794</v>
       </c>
       <c r="F344" t="n">
         <v>-0.136562</v>
@@ -10067,7 +10067,7 @@
         <v>1.636514588996994</v>
       </c>
       <c r="E345" t="n">
-        <v>0.09953193845103182</v>
+        <v>5.70276</v>
       </c>
       <c r="F345" t="n">
         <v>-0.100586</v>
@@ -10095,7 +10095,7 @@
         <v>1.616786937107051</v>
       </c>
       <c r="E346" t="n">
-        <v>0.1022405149172018</v>
+        <v>5.85795</v>
       </c>
       <c r="F346" t="n">
         <v>-0.009359849999999999</v>
@@ -10123,7 +10123,7 @@
         <v>1.590204389378925</v>
       </c>
       <c r="E347" t="n">
-        <v>0.1060339880464115</v>
+        <v>6.0753</v>
       </c>
       <c r="F347" t="n">
         <v>-0.259811</v>
@@ -10151,7 +10151,7 @@
         <v>1.681356595133822</v>
       </c>
       <c r="E348" t="n">
-        <v>0.001603498560989514</v>
+        <v>0.0918737</v>
       </c>
       <c r="F348" t="n">
         <v>-0.034697</v>
@@ -10179,7 +10179,7 @@
         <v>1.686223591342501</v>
       </c>
       <c r="E349" t="n">
-        <v>0.004861754257770364</v>
+        <v>0.278558</v>
       </c>
       <c r="F349" t="n">
         <v>0.0934845</v>
@@ -10207,7 +10207,7 @@
         <v>1.735655495770978</v>
       </c>
       <c r="E350" t="n">
-        <v>0.008044554134999745</v>
+        <v>0.460919</v>
       </c>
       <c r="F350" t="n">
         <v>-0.000849172</v>
@@ -10235,7 +10235,7 @@
         <v>1.722654927720581</v>
       </c>
       <c r="E351" t="n">
-        <v>0.01381545040013396</v>
+        <v>0.791567</v>
       </c>
       <c r="F351" t="n">
         <v>0.438559</v>
@@ -10263,7 +10263,7 @@
         <v>1.700576372880677</v>
       </c>
       <c r="E352" t="n">
-        <v>0.02724825481506067</v>
+        <v>1.56121</v>
       </c>
       <c r="F352" t="n">
         <v>0.401293</v>
@@ -10291,7 +10291,7 @@
         <v>1.668691103829585</v>
       </c>
       <c r="E353" t="n">
-        <v>0.03628556968188731</v>
+        <v>2.07901</v>
       </c>
       <c r="F353" t="n">
         <v>0.235735</v>
@@ -10319,7 +10319,7 @@
         <v>1.665148642013679</v>
       </c>
       <c r="E354" t="n">
-        <v>0.04418405721178765</v>
+        <v>2.53156</v>
       </c>
       <c r="F354" t="n">
         <v>0.136015</v>
@@ -10347,7 +10347,7 @@
         <v>1.667291216314654</v>
       </c>
       <c r="E355" t="n">
-        <v>0.04923783259386243</v>
+        <v>2.82112</v>
       </c>
       <c r="F355" t="n">
         <v>0.10617</v>
@@ -10375,7 +10375,7 @@
         <v>1.665001501500824</v>
       </c>
       <c r="E356" t="n">
-        <v>0.0555861186821414</v>
+        <v>3.18485</v>
       </c>
       <c r="F356" t="n">
         <v>0.0225519</v>
@@ -10403,7 +10403,7 @@
         <v>1.655533146753637</v>
       </c>
       <c r="E357" t="n">
-        <v>0.06301773063713326</v>
+        <v>3.61065</v>
       </c>
       <c r="F357" t="n">
         <v>-0.0898755</v>
@@ -10431,7 +10431,7 @@
         <v>1.69450582766776</v>
       </c>
       <c r="E358" t="n">
-        <v>0.0728544063013733</v>
+        <v>4.17425</v>
       </c>
       <c r="F358" t="n">
         <v>-0.12863</v>
@@ -10459,7 +10459,7 @@
         <v>1.683977434528147</v>
       </c>
       <c r="E359" t="n">
-        <v>0.08346583362057362</v>
+        <v>4.78224</v>
       </c>
       <c r="F359" t="n">
         <v>-0.453458</v>
@@ -10487,7 +10487,7 @@
         <v>1.672820970695908</v>
       </c>
       <c r="E360" t="n">
-        <v>0.09133081082883568</v>
+        <v>5.23287</v>
       </c>
       <c r="F360" t="n">
         <v>-0.319984</v>
@@ -10515,7 +10515,7 @@
         <v>1.689346027313528</v>
       </c>
       <c r="E361" t="n">
-        <v>0.09662491804891007</v>
+        <v>5.5362</v>
       </c>
       <c r="F361" t="n">
         <v>-0.12087</v>
@@ -10543,7 +10543,7 @@
         <v>1.74031031715611</v>
       </c>
       <c r="E362" t="n">
-        <v>0.1006257362932567</v>
+        <v>5.76543</v>
       </c>
       <c r="F362" t="n">
         <v>-0.141204</v>
@@ -10571,7 +10571,7 @@
         <v>1.695520569028875</v>
       </c>
       <c r="E363" t="n">
-        <v>0.1036648781197544</v>
+        <v>5.93956</v>
       </c>
       <c r="F363" t="n">
         <v>0.0147439</v>
@@ -10599,7 +10599,7 @@
         <v>1.676162283312687</v>
       </c>
       <c r="E364" t="n">
-        <v>0.1074347893040622</v>
+        <v>6.15556</v>
       </c>
       <c r="F364" t="n">
         <v>0.00049997</v>
@@ -10627,7 +10627,7 @@
         <v>1.701043797202177</v>
       </c>
       <c r="E365" t="n">
-        <v>0.004690397831809561</v>
+        <v>0.26874</v>
       </c>
       <c r="F365" t="n">
         <v>0.423499</v>
@@ -10655,7 +10655,7 @@
         <v>1.715671880051661</v>
       </c>
       <c r="E366" t="n">
-        <v>0.01574843745330272</v>
+        <v>0.902319</v>
       </c>
       <c r="F366" t="n">
         <v>0.0775368</v>
@@ -10683,7 +10683,7 @@
         <v>1.677071852962776</v>
       </c>
       <c r="E367" t="n">
-        <v>0.02804534668444648</v>
+        <v>1.60688</v>
       </c>
       <c r="F367" t="n">
         <v>0.674695</v>
@@ -10711,7 +10711,7 @@
         <v>1.700999706055236</v>
       </c>
       <c r="E368" t="n">
-        <v>0.03823772045024296</v>
+        <v>2.19086</v>
       </c>
       <c r="F368" t="n">
         <v>-0.442036</v>
@@ -10739,7 +10739,7 @@
         <v>1.70489882397754</v>
       </c>
       <c r="E369" t="n">
-        <v>0.04836935675807005</v>
+        <v>2.77136</v>
       </c>
       <c r="F369" t="n">
         <v>-0.117168</v>
@@ -10767,7 +10767,7 @@
         <v>1.694980825850251</v>
       </c>
       <c r="E370" t="n">
-        <v>0.06015032920903177</v>
+        <v>3.44636</v>
       </c>
       <c r="F370" t="n">
         <v>0.0988903</v>
@@ -10795,7 +10795,7 @@
         <v>1.689126993449575</v>
       </c>
       <c r="E371" t="n">
-        <v>0.07175223087873889</v>
+        <v>4.1111</v>
       </c>
       <c r="F371" t="n">
         <v>0.34059</v>
@@ -10823,7 +10823,7 @@
         <v>1.704596726501609</v>
       </c>
       <c r="E372" t="n">
-        <v>0.1059697599299381</v>
+        <v>6.07162</v>
       </c>
       <c r="F372" t="n">
         <v>-0.11512</v>
@@ -10851,7 +10851,7 @@
         <v>1.678162685796583</v>
       </c>
       <c r="E373" t="n">
-        <v>0.002411887946623484</v>
+        <v>0.138191</v>
       </c>
       <c r="F373" t="n">
         <v>0.0763109</v>
@@ -10879,7 +10879,7 @@
         <v>1.703226350195417</v>
       </c>
       <c r="E374" t="n">
-        <v>0.006151412948654014</v>
+        <v>0.35245</v>
       </c>
       <c r="F374" t="n">
         <v>0.0580808</v>
@@ -10907,7 +10907,7 @@
         <v>1.69656712216169</v>
       </c>
       <c r="E375" t="n">
-        <v>0.01075784299015013</v>
+        <v>0.616379</v>
       </c>
       <c r="F375" t="n">
         <v>-0.0637202</v>
@@ -10935,7 +10935,7 @@
         <v>1.676257736745755</v>
       </c>
       <c r="E376" t="n">
-        <v>0.02004248846527688</v>
+        <v>1.14835</v>
       </c>
       <c r="F376" t="n">
         <v>0.0330118</v>
@@ -10963,7 +10963,7 @@
         <v>1.667848914020692</v>
       </c>
       <c r="E377" t="n">
-        <v>0.0437679707181122</v>
+        <v>2.50772</v>
       </c>
       <c r="F377" t="n">
         <v>0.0764736</v>
@@ -10991,7 +10991,7 @@
         <v>1.659677679551063</v>
       </c>
       <c r="E378" t="n">
-        <v>0.05278329443636371</v>
+        <v>3.02426</v>
       </c>
       <c r="F378" t="n">
         <v>-0.185095</v>
@@ -11019,7 +11019,7 @@
         <v>1.680981855940153</v>
       </c>
       <c r="E379" t="n">
-        <v>0.063158404174844</v>
+        <v>3.61871</v>
       </c>
       <c r="F379" t="n">
         <v>0.217827</v>
@@ -11047,7 +11047,7 @@
         <v>1.697477540352154</v>
       </c>
       <c r="E380" t="n">
-        <v>0.077688444730622</v>
+        <v>4.45122</v>
       </c>
       <c r="F380" t="n">
         <v>-0.392929</v>
@@ -11075,7 +11075,7 @@
         <v>1.682028537213326</v>
       </c>
       <c r="E381" t="n">
-        <v>0.08489944706816176</v>
+        <v>4.86438</v>
       </c>
       <c r="F381" t="n">
         <v>0.0457497</v>
@@ -11103,7 +11103,7 @@
         <v>1.673538168073857</v>
       </c>
       <c r="E382" t="n">
-        <v>0.09362120640622783</v>
+        <v>5.3641</v>
       </c>
       <c r="F382" t="n">
         <v>-0.129018</v>
@@ -11131,7 +11131,7 @@
         <v>1.700382309952676</v>
       </c>
       <c r="E383" t="n">
-        <v>0.101152825727359</v>
+        <v>5.79563</v>
       </c>
       <c r="F383" t="n">
         <v>0.00139381</v>
@@ -11159,7 +11159,7 @@
         <v>1.679877971758663</v>
       </c>
       <c r="E384" t="n">
-        <v>0.1045225329141844</v>
+        <v>5.9887</v>
       </c>
       <c r="F384" t="n">
         <v>-0.0868313</v>
@@ -11187,7 +11187,7 @@
         <v>1.673786127317346</v>
       </c>
       <c r="E385" t="n">
-        <v>0.1080149367474251</v>
+        <v>6.1888</v>
       </c>
       <c r="F385" t="n">
         <v>-0.044697</v>
@@ -11215,7 +11215,7 @@
         <v>1.879898933453604</v>
       </c>
       <c r="E386" t="n">
-        <v>0.001501129764372291</v>
+        <v>0.0860084</v>
       </c>
       <c r="F386" t="n">
         <v>0.009097849999999999</v>
@@ -11243,7 +11243,7 @@
         <v>1.882968401221858</v>
       </c>
       <c r="E387" t="n">
-        <v>0.004898179279259486</v>
+        <v>0.280645</v>
       </c>
       <c r="F387" t="n">
         <v>0.0765629</v>
@@ -11271,7 +11271,7 @@
         <v>1.885908269243231</v>
       </c>
       <c r="E388" t="n">
-        <v>0.008046264557666698</v>
+        <v>0.461017</v>
       </c>
       <c r="F388" t="n">
         <v>-0.080779</v>
@@ -11299,7 +11299,7 @@
         <v>1.898170171507286</v>
       </c>
       <c r="E389" t="n">
-        <v>0.01180994491654483</v>
+        <v>0.67666</v>
       </c>
       <c r="F389" t="n">
         <v>0.0938286</v>
@@ -11327,7 +11327,7 @@
         <v>1.903630741504245</v>
       </c>
       <c r="E390" t="n">
-        <v>0.01683860501068341</v>
+        <v>0.964781</v>
       </c>
       <c r="F390" t="n">
         <v>0.254069</v>
@@ -11355,7 +11355,7 @@
         <v>1.909929318063891</v>
       </c>
       <c r="E391" t="n">
-        <v>0.02326715879126161</v>
+        <v>1.33311</v>
       </c>
       <c r="F391" t="n">
         <v>0.292508</v>
@@ -11383,7 +11383,7 @@
         <v>1.917858180366838</v>
       </c>
       <c r="E392" t="n">
-        <v>0.02932606928955992</v>
+        <v>1.68026</v>
       </c>
       <c r="F392" t="n">
         <v>-0.0380433</v>
@@ -11411,7 +11411,7 @@
         <v>1.902711223491363</v>
       </c>
       <c r="E393" t="n">
-        <v>0.03787015410977296</v>
+        <v>2.1698</v>
       </c>
       <c r="F393" t="n">
         <v>0.246959</v>
@@ -11439,7 +11439,7 @@
         <v>1.93011139574896</v>
       </c>
       <c r="E394" t="n">
-        <v>0.04984328731137926</v>
+        <v>2.85581</v>
       </c>
       <c r="F394" t="n">
         <v>-0.136657</v>
@@ -11467,7 +11467,7 @@
         <v>1.939762872105763</v>
       </c>
       <c r="E395" t="n">
-        <v>0.08321590247168804</v>
+        <v>4.76792</v>
       </c>
       <c r="F395" t="n">
         <v>-0.214695</v>
@@ -11495,7 +11495,7 @@
         <v>1.885709415578127</v>
       </c>
       <c r="E396" t="n">
-        <v>0.09422561392619345</v>
+        <v>5.39873</v>
       </c>
       <c r="F396" t="n">
         <v>-0.312336</v>
@@ -11523,7 +11523,7 @@
         <v>1.874651967699605</v>
       </c>
       <c r="E397" t="n">
-        <v>0.1019654510270875</v>
+        <v>5.84219</v>
       </c>
       <c r="F397" t="n">
         <v>-0.0767539</v>
@@ -11551,7 +11551,7 @@
         <v>1.87564922093658</v>
       </c>
       <c r="E398" t="n">
-        <v>0.1070930538365217</v>
+        <v>6.13598</v>
       </c>
       <c r="F398" t="n">
         <v>0.168548</v>
@@ -11579,7 +11579,7 @@
         <v>2.013606217709908</v>
       </c>
       <c r="E399" t="n">
-        <v>0.001647636192443199</v>
+        <v>0.0944026</v>
       </c>
       <c r="F399" t="n">
         <v>3.35106e-05</v>
@@ -11607,7 +11607,7 @@
         <v>2.004936407969091</v>
       </c>
       <c r="E400" t="n">
-        <v>0.004911391421697083</v>
+        <v>0.281402</v>
       </c>
       <c r="F400" t="n">
         <v>0.314291</v>
@@ -11635,7 +11635,7 @@
         <v>1.998594506146757</v>
       </c>
       <c r="E401" t="n">
-        <v>0.008387790585696948</v>
+        <v>0.480585</v>
       </c>
       <c r="F401" t="n">
         <v>0.09403880000000001</v>
@@ -11663,7 +11663,7 @@
         <v>1.985492382256855</v>
       </c>
       <c r="E402" t="n">
-        <v>0.01147049583032445</v>
+        <v>0.657211</v>
       </c>
       <c r="F402" t="n">
         <v>0.226174</v>
@@ -11691,7 +11691,7 @@
         <v>2.013794925010985</v>
       </c>
       <c r="E403" t="n">
-        <v>0.014775084782758</v>
+        <v>0.84655</v>
       </c>
       <c r="F403" t="n">
         <v>-0.0946389</v>
@@ -11719,7 +11719,7 @@
         <v>2.023358594021337</v>
       </c>
       <c r="E404" t="n">
-        <v>0.01824165774306913</v>
+        <v>1.04517</v>
       </c>
       <c r="F404" t="n">
         <v>0.213834</v>
@@ -11747,7 +11747,7 @@
         <v>2.032390218437394</v>
       </c>
       <c r="E405" t="n">
-        <v>0.02180806353659434</v>
+        <v>1.24951</v>
       </c>
       <c r="F405" t="n">
         <v>0.375281</v>
@@ -11775,7 +11775,7 @@
         <v>2.003821349322339</v>
       </c>
       <c r="E406" t="n">
-        <v>0.02615829669719022</v>
+        <v>1.49876</v>
       </c>
       <c r="F406" t="n">
         <v>-0.0571195</v>
@@ -11803,7 +11803,7 @@
         <v>2.028484656091833</v>
       </c>
       <c r="E407" t="n">
-        <v>0.03176918117650158</v>
+        <v>1.82024</v>
       </c>
       <c r="F407" t="n">
         <v>0.182147</v>
@@ -11831,7 +11831,7 @@
         <v>2.04130595453009</v>
       </c>
       <c r="E408" t="n">
-        <v>0.03906902077296787</v>
+        <v>2.23849</v>
       </c>
       <c r="F408" t="n">
         <v>0.503252</v>
@@ -11859,7 +11859,7 @@
         <v>2.042309966679887</v>
       </c>
       <c r="E409" t="n">
-        <v>0.0520806248795108</v>
+        <v>2.984</v>
       </c>
       <c r="F409" t="n">
         <v>-0.192655</v>
@@ -11887,7 +11887,7 @@
         <v>2.022342700928802</v>
       </c>
       <c r="E410" t="n">
-        <v>0.06380173253712912</v>
+        <v>3.65557</v>
       </c>
       <c r="F410" t="n">
         <v>-0.150663</v>
@@ -11915,7 +11915,7 @@
         <v>2.05961889678649</v>
       </c>
       <c r="E411" t="n">
-        <v>0.07348150310161487</v>
+        <v>4.21018</v>
       </c>
       <c r="F411" t="n">
         <v>-0.141813</v>
@@ -11943,7 +11943,7 @@
         <v>2.033708435346621</v>
       </c>
       <c r="E412" t="n">
-        <v>0.08353128346752341</v>
+        <v>4.78599</v>
       </c>
       <c r="F412" t="n">
         <v>-0.315948</v>
@@ -11971,7 +11971,7 @@
         <v>2.02076223242617</v>
       </c>
       <c r="E413" t="n">
-        <v>0.09068783153240097</v>
+        <v>5.19603</v>
       </c>
       <c r="F413" t="n">
         <v>-0.229825</v>
@@ -11999,7 +11999,7 @@
         <v>2.00155939207409</v>
       </c>
       <c r="E414" t="n">
-        <v>0.09732828573746378</v>
+        <v>5.5765</v>
       </c>
       <c r="F414" t="n">
         <v>-0.171718</v>
@@ -12027,7 +12027,7 @@
         <v>2.005265568447232</v>
       </c>
       <c r="E415" t="n">
-        <v>0.101387397978827</v>
+        <v>5.80907</v>
       </c>
       <c r="F415" t="n">
         <v>-0.203184</v>
@@ -12055,7 +12055,7 @@
         <v>2.00066988781258</v>
       </c>
       <c r="E416" t="n">
-        <v>0.1048014365286531</v>
+        <v>6.00468</v>
       </c>
       <c r="F416" t="n">
         <v>0.0355288</v>
@@ -12083,7 +12083,7 @@
         <v>2.019806921465515</v>
       </c>
       <c r="E417" t="n">
-        <v>0.1080051629036139</v>
+        <v>6.18824</v>
       </c>
       <c r="F417" t="n">
         <v>0.0271083</v>
@@ -12111,7 +12111,7 @@
         <v>1.935892559002178</v>
       </c>
       <c r="E418" t="n">
-        <v>0.001654844402253936</v>
+        <v>0.0948156</v>
       </c>
       <c r="F418" t="n">
         <v>0.0373978</v>
@@ -12139,7 +12139,7 @@
         <v>1.927270090049654</v>
       </c>
       <c r="E419" t="n">
-        <v>0.004874111188874484</v>
+        <v>0.279266</v>
       </c>
       <c r="F419" t="n">
         <v>0.06534710000000001</v>
@@ -12167,7 +12167,7 @@
         <v>1.899721032151826</v>
       </c>
       <c r="E420" t="n">
-        <v>0.0079535003079232</v>
+        <v>0.455702</v>
       </c>
       <c r="F420" t="n">
         <v>0.0499035</v>
@@ -12195,7 +12195,7 @@
         <v>1.878030883665122</v>
       </c>
       <c r="E421" t="n">
-        <v>0.01128931320067492</v>
+        <v>0.64683</v>
       </c>
       <c r="F421" t="n">
         <v>0.197284</v>
@@ -12223,7 +12223,7 @@
         <v>1.914886419608223</v>
       </c>
       <c r="E422" t="n">
-        <v>0.01713747519179492</v>
+        <v>0.981905</v>
       </c>
       <c r="F422" t="n">
         <v>0.241219</v>
@@ -12251,7 +12251,7 @@
         <v>1.95157884800999</v>
       </c>
       <c r="E423" t="n">
-        <v>0.02312753245110206</v>
+        <v>1.32511</v>
       </c>
       <c r="F423" t="n">
         <v>0.246178</v>
@@ -12279,7 +12279,7 @@
         <v>1.944091047250617</v>
       </c>
       <c r="E424" t="n">
-        <v>0.02769977149255161</v>
+        <v>1.58708</v>
       </c>
       <c r="F424" t="n">
         <v>0.249966</v>
@@ -12307,7 +12307,7 @@
         <v>1.933540793466742</v>
       </c>
       <c r="E425" t="n">
-        <v>0.03422032157800242</v>
+        <v>1.96068</v>
       </c>
       <c r="F425" t="n">
         <v>0.294239</v>
@@ -12335,7 +12335,7 @@
         <v>1.91654898189428</v>
       </c>
       <c r="E426" t="n">
-        <v>0.04218216455975015</v>
+        <v>2.41686</v>
       </c>
       <c r="F426" t="n">
         <v>0.111382</v>
@@ -12363,7 +12363,7 @@
         <v>1.924375223286768</v>
       </c>
       <c r="E427" t="n">
-        <v>0.05041191558167901</v>
+        <v>2.88839</v>
       </c>
       <c r="F427" t="n">
         <v>0.077052</v>
@@ -12391,7 +12391,7 @@
         <v>1.917769537770376</v>
       </c>
       <c r="E428" t="n">
-        <v>0.05781560226863897</v>
+        <v>3.31259</v>
       </c>
       <c r="F428" t="n">
         <v>0.0419381</v>
@@ -12419,7 +12419,7 @@
         <v>1.915476442037333</v>
       </c>
       <c r="E429" t="n">
-        <v>0.06803537770369177</v>
+        <v>3.89814</v>
       </c>
       <c r="F429" t="n">
         <v>-0.176937</v>
@@ -12447,7 +12447,7 @@
         <v>1.929181173451576</v>
       </c>
       <c r="E430" t="n">
-        <v>0.07995370756678544</v>
+        <v>4.58101</v>
       </c>
       <c r="F430" t="n">
         <v>-0.160944</v>
@@ -12475,7 +12475,7 @@
         <v>1.945613013936739</v>
       </c>
       <c r="E431" t="n">
-        <v>0.0890152825102148</v>
+        <v>5.1002</v>
       </c>
       <c r="F431" t="n">
         <v>-0.237468</v>
@@ -12503,7 +12503,7 @@
         <v>1.885836684339341</v>
       </c>
       <c r="E432" t="n">
-        <v>0.09937485881835234</v>
+        <v>5.69376</v>
       </c>
       <c r="F432" t="n">
         <v>-0.211262</v>
@@ -12531,7 +12531,7 @@
         <v>1.916723767265383</v>
       </c>
       <c r="E433" t="n">
-        <v>0.1026482238304677</v>
+        <v>5.88131</v>
       </c>
       <c r="F433" t="n">
         <v>-0.129254</v>
@@ -12559,7 +12559,7 @@
         <v>1.934623994475412</v>
       </c>
       <c r="E434" t="n">
-        <v>0.1069867632850752</v>
+        <v>6.12989</v>
       </c>
       <c r="F434" t="n">
         <v>-0.140436</v>
@@ -12587,7 +12587,7 @@
         <v>1.988102110053706</v>
       </c>
       <c r="E435" t="n">
-        <v>0.001640401802693682</v>
+        <v>0.0939881</v>
       </c>
       <c r="F435" t="n">
         <v>0.0498468</v>
@@ -12615,7 +12615,7 @@
         <v>1.97365397169818</v>
       </c>
       <c r="E436" t="n">
-        <v>0.005040685412684823</v>
+        <v>0.28881</v>
       </c>
       <c r="F436" t="n">
         <v>-0.0354157</v>
@@ -12643,7 +12643,7 @@
         <v>2.000394961001452</v>
       </c>
       <c r="E437" t="n">
-        <v>0.008280068864263858</v>
+        <v>0.474413</v>
       </c>
       <c r="F437" t="n">
         <v>0.282301</v>
@@ -12671,7 +12671,7 @@
         <v>2.008118522398516</v>
       </c>
       <c r="E438" t="n">
-        <v>0.01198419858906394</v>
+        <v>0.686644</v>
       </c>
       <c r="F438" t="n">
         <v>0.332003</v>
@@ -12699,7 +12699,7 @@
         <v>2.007966633188909</v>
       </c>
       <c r="E439" t="n">
-        <v>0.01631877614626942</v>
+        <v>0.934997</v>
       </c>
       <c r="F439" t="n">
         <v>0.113569</v>
@@ -12727,7 +12727,7 @@
         <v>2.030438376311874</v>
       </c>
       <c r="E440" t="n">
-        <v>0.02308878614170778</v>
+        <v>1.32289</v>
       </c>
       <c r="F440" t="n">
         <v>0.452099</v>
@@ -12755,7 +12755,7 @@
         <v>2.021816015368362</v>
       </c>
       <c r="E441" t="n">
-        <v>0.03202836257042274</v>
+        <v>1.83509</v>
       </c>
       <c r="F441" t="n">
         <v>0.276031</v>
@@ -12783,7 +12783,7 @@
         <v>2.010758563328775</v>
       </c>
       <c r="E442" t="n">
-        <v>0.04059670746723851</v>
+        <v>2.32602</v>
       </c>
       <c r="F442" t="n">
         <v>0.28401</v>
@@ -12811,7 +12811,7 @@
         <v>2.04458308708646</v>
       </c>
       <c r="E443" t="n">
-        <v>0.05421079923156988</v>
+        <v>3.10605</v>
       </c>
       <c r="F443" t="n">
         <v>0.256107</v>
@@ -12839,7 +12839,7 @@
         <v>2.000104997243895</v>
       </c>
       <c r="E444" t="n">
-        <v>0.06246865005445584</v>
+        <v>3.57919</v>
       </c>
       <c r="F444" t="n">
         <v>0.0303533</v>
@@ -12867,7 +12867,7 @@
         <v>2.016033233853054</v>
       </c>
       <c r="E445" t="n">
-        <v>0.07384749864575808</v>
+        <v>4.23115</v>
       </c>
       <c r="F445" t="n">
         <v>-0.148224</v>
@@ -12895,7 +12895,7 @@
         <v>2.035165840908303</v>
       </c>
       <c r="E446" t="n">
-        <v>0.08610005906060866</v>
+        <v>4.93317</v>
       </c>
       <c r="F446" t="n">
         <v>-0.29156</v>
@@ -12923,7 +12923,7 @@
         <v>2.018110502425474</v>
       </c>
       <c r="E447" t="n">
-        <v>0.09711867169429927</v>
+        <v>5.56449</v>
       </c>
       <c r="F447" t="n">
         <v>-0.203253</v>
@@ -12951,7 +12951,7 @@
         <v>1.99572543201714</v>
       </c>
       <c r="E448" t="n">
-        <v>0.1033210482571115</v>
+        <v>5.91986</v>
       </c>
       <c r="F448" t="n">
         <v>-0.126303</v>
@@ -12979,7 +12979,7 @@
         <v>2.002920367862886</v>
       </c>
       <c r="E449" t="n">
-        <v>0.1074815641280156</v>
+        <v>6.15824</v>
       </c>
       <c r="F449" t="n">
         <v>-0.0249437</v>
@@ -13007,7 +13007,7 @@
         <v>1.964940202652488</v>
       </c>
       <c r="E450" t="n">
-        <v>0.001621161293019697</v>
+        <v>0.0928857</v>
       </c>
       <c r="F450" t="n">
         <v>0.0734173</v>
@@ -13035,7 +13035,7 @@
         <v>1.971783456670636</v>
       </c>
       <c r="E451" t="n">
-        <v>0.004998221551983801</v>
+        <v>0.286377</v>
       </c>
       <c r="F451" t="n">
         <v>0.021175</v>
@@ -13063,7 +13063,7 @@
         <v>1.948235098749635</v>
       </c>
       <c r="E452" t="n">
-        <v>0.008077017259086838</v>
+        <v>0.462779</v>
       </c>
       <c r="F452" t="n">
         <v>0.128221</v>
@@ -13091,7 +13091,7 @@
         <v>1.909146406119761</v>
       </c>
       <c r="E453" t="n">
-        <v>0.01151915560987006</v>
+        <v>0.659999</v>
       </c>
       <c r="F453" t="n">
         <v>0.255115</v>
@@ -13119,7 +13119,7 @@
         <v>1.937924147122379</v>
       </c>
       <c r="E454" t="n">
-        <v>0.02306190807122708</v>
+        <v>1.32135</v>
       </c>
       <c r="F454" t="n">
         <v>0.450857</v>
@@ -13147,7 +13147,7 @@
         <v>1.949784603488293</v>
       </c>
       <c r="E455" t="n">
-        <v>0.03369986439505771</v>
+        <v>1.93086</v>
       </c>
       <c r="F455" t="n">
         <v>0.300586</v>
@@ -13175,7 +13175,7 @@
         <v>1.932058487727533</v>
       </c>
       <c r="E456" t="n">
-        <v>0.04413920225001139</v>
+        <v>2.52899</v>
       </c>
       <c r="F456" t="n">
         <v>-0.111614</v>
@@ -13203,7 +13203,7 @@
         <v>1.946186013720169</v>
       </c>
       <c r="E457" t="n">
-        <v>0.05281436129704921</v>
+        <v>3.02604</v>
       </c>
       <c r="F457" t="n">
         <v>0.145767</v>
@@ -13231,7 +13231,7 @@
         <v>1.911836813119781</v>
       </c>
       <c r="E458" t="n">
-        <v>0.06417069514100071</v>
+        <v>3.67671</v>
       </c>
       <c r="F458" t="n">
         <v>0.11351</v>
@@ -13259,7 +13259,7 @@
         <v>1.931817796791405</v>
       </c>
       <c r="E459" t="n">
-        <v>0.07654298514253811</v>
+        <v>4.38559</v>
       </c>
       <c r="F459" t="n">
         <v>-0.229764</v>
@@ -13287,7 +13287,7 @@
         <v>1.934352604878438</v>
       </c>
       <c r="E460" t="n">
-        <v>0.08485947902829111</v>
+        <v>4.86209</v>
       </c>
       <c r="F460" t="n">
         <v>-0.0430121</v>
@@ -13315,7 +13315,7 @@
         <v>1.914737579930994</v>
       </c>
       <c r="E461" t="n">
-        <v>0.0945228434978081</v>
+        <v>5.41576</v>
       </c>
       <c r="F461" t="n">
         <v>-0.287994</v>
@@ -13343,7 +13343,7 @@
         <v>1.927117017723625</v>
       </c>
       <c r="E462" t="n">
-        <v>0.1006466802442806</v>
+        <v>5.76663</v>
       </c>
       <c r="F462" t="n">
         <v>-0.158315</v>
@@ -13371,7 +13371,7 @@
         <v>1.960635101185328</v>
       </c>
       <c r="E463" t="n">
-        <v>0.1035004681042165</v>
+        <v>5.93014</v>
       </c>
       <c r="F463" t="n">
         <v>-0.121095</v>
@@ -13399,7 +13399,7 @@
         <v>1.967648342565307</v>
       </c>
       <c r="E464" t="n">
-        <v>0.1072794550006347</v>
+        <v>6.14666</v>
       </c>
       <c r="F464" t="n">
         <v>0.00338064</v>
@@ -13427,7 +13427,7 @@
         <v>2.064020348736901</v>
       </c>
       <c r="E465" t="n">
-        <v>0.00146194014134801</v>
+        <v>0.083763</v>
       </c>
       <c r="F465" t="n">
         <v>0.0484245</v>
@@ -13455,7 +13455,7 @@
         <v>2.048826493385909</v>
       </c>
       <c r="E466" t="n">
-        <v>0.004793773683405185</v>
+        <v>0.274663</v>
       </c>
       <c r="F466" t="n">
         <v>0.242801</v>
@@ -13483,7 +13483,7 @@
         <v>2.022468788387104</v>
       </c>
       <c r="E467" t="n">
-        <v>0.008277485776970907</v>
+        <v>0.474265</v>
       </c>
       <c r="F467" t="n">
         <v>0.0249318</v>
@@ -13511,7 +13511,7 @@
         <v>2.027597100017654</v>
       </c>
       <c r="E468" t="n">
-        <v>0.01420083655226682</v>
+        <v>0.813648</v>
       </c>
       <c r="F468" t="n">
         <v>0.253094</v>
@@ -13539,7 +13539,7 @@
         <v>2.01086548530726</v>
       </c>
       <c r="E469" t="n">
-        <v>0.02532996343419371</v>
+        <v>1.4513</v>
       </c>
       <c r="F469" t="n">
         <v>0.115324</v>
@@ -13567,7 +13567,7 @@
         <v>2.030059112439832</v>
       </c>
       <c r="E470" t="n">
-        <v>0.03445611555994686</v>
+        <v>1.97419</v>
       </c>
       <c r="F470" t="n">
         <v>0.0965134</v>
@@ -13595,7 +13595,7 @@
         <v>1.996266515272948</v>
       </c>
       <c r="E471" t="n">
-        <v>0.04246996935340402</v>
+        <v>2.43335</v>
       </c>
       <c r="F471" t="n">
         <v>-0.0613049</v>
@@ -13623,7 +13623,7 @@
         <v>1.997693670210726</v>
       </c>
       <c r="E472" t="n">
-        <v>0.05104267757334977</v>
+        <v>2.92453</v>
       </c>
       <c r="F472" t="n">
         <v>-0.00829656</v>
@@ -13651,7 +13651,7 @@
         <v>2.017719009178434</v>
       </c>
       <c r="E473" t="n">
-        <v>0.06116331830688929</v>
+        <v>3.5044</v>
       </c>
       <c r="F473" t="n">
         <v>0.142732</v>
@@ -13679,7 +13679,7 @@
         <v>1.997688664431973</v>
       </c>
       <c r="E474" t="n">
-        <v>0.07214754795431561</v>
+        <v>4.13375</v>
       </c>
       <c r="F474" t="n">
         <v>-0.599993</v>
@@ -13707,7 +13707,7 @@
         <v>2.042153275344434</v>
       </c>
       <c r="E475" t="n">
-        <v>0.08295689561069207</v>
+        <v>4.75308</v>
       </c>
       <c r="F475" t="n">
         <v>-0.596868</v>
@@ -13735,7 +13735,7 @@
         <v>2.032274587746449</v>
       </c>
       <c r="E476" t="n">
-        <v>0.0936903214446068</v>
+        <v>5.36806</v>
       </c>
       <c r="F476" t="n">
         <v>-0.228192</v>
@@ -13763,7 +13763,7 @@
         <v>2.06351157011537</v>
       </c>
       <c r="E477" t="n">
-        <v>0.1039832261753182</v>
+        <v>5.9578</v>
       </c>
       <c r="F477" t="n">
         <v>-0.18235</v>
@@ -13791,7 +13791,7 @@
         <v>2.051228899952416</v>
       </c>
       <c r="E478" t="n">
-        <v>0.1079964362573539</v>
+        <v>6.18774</v>
       </c>
       <c r="F478" t="n">
         <v>-0.0878935</v>
@@ -13819,7 +13819,7 @@
         <v>1.929012700839474</v>
       </c>
       <c r="E479" t="n">
-        <v>0.004299321906315191</v>
+        <v>0.246333</v>
       </c>
       <c r="F479" t="n">
         <v>0.130053</v>
@@ -13847,7 +13847,7 @@
         <v>1.963035914088176</v>
       </c>
       <c r="E480" t="n">
-        <v>0.00800556347951019</v>
+        <v>0.458685</v>
       </c>
       <c r="F480" t="n">
         <v>0.179863</v>
@@ -13875,7 +13875,7 @@
         <v>1.934140636044856</v>
       </c>
       <c r="E481" t="n">
-        <v>0.01491031289320252</v>
+        <v>0.854298</v>
       </c>
       <c r="F481" t="n">
         <v>-0.0336346</v>
@@ -13903,7 +13903,7 @@
         <v>1.943154651591067</v>
       </c>
       <c r="E482" t="n">
-        <v>0.04814176582360999</v>
+        <v>2.75832</v>
       </c>
       <c r="F482" t="n">
         <v>-0.0455624</v>
@@ -13931,7 +13931,7 @@
         <v>1.944731343913601</v>
       </c>
       <c r="E483" t="n">
-        <v>0.08121086822699695</v>
+        <v>4.65304</v>
       </c>
       <c r="F483" t="n">
         <v>-0.337294</v>
@@ -13959,7 +13959,7 @@
         <v>1.934688605434993</v>
       </c>
       <c r="E484" t="n">
-        <v>0.09068940232872776</v>
+        <v>5.19612</v>
       </c>
       <c r="F484" t="n">
         <v>0.100837</v>
@@ -13987,7 +13987,7 @@
         <v>1.953171779439791</v>
       </c>
       <c r="E485" t="n">
-        <v>0.1006679732611549</v>
+        <v>5.76785</v>
       </c>
       <c r="F485" t="n">
         <v>-0.313852</v>
@@ -14015,7 +14015,7 @@
         <v>1.941520023074704</v>
       </c>
       <c r="E486" t="n">
-        <v>0.1034419995742747</v>
+        <v>5.92679</v>
       </c>
       <c r="F486" t="n">
         <v>-0.0910101</v>
@@ -14043,7 +14043,7 @@
         <v>1.913115260510981</v>
       </c>
       <c r="E487" t="n">
-        <v>0.1070485479405958</v>
+        <v>6.13343</v>
       </c>
       <c r="F487" t="n">
         <v>0.0248133</v>
@@ -14071,7 +14071,7 @@
         <v>2.061516432144066</v>
       </c>
       <c r="E488" t="n">
-        <v>0.002118044313757719</v>
+        <v>0.121355</v>
       </c>
       <c r="F488" t="n">
         <v>-0.0031007</v>
@@ -14099,7 +14099,7 @@
         <v>2.099714266275295</v>
       </c>
       <c r="E489" t="n">
-        <v>0.00729767538819381</v>
+        <v>0.418126</v>
       </c>
       <c r="F489" t="n">
         <v>0.268048</v>
@@ -14127,7 +14127,7 @@
         <v>2.053280302345493</v>
       </c>
       <c r="E490" t="n">
-        <v>0.02084184926269029</v>
+        <v>1.19415</v>
       </c>
       <c r="F490" t="n">
         <v>-0.0239659</v>
@@ -14155,7 +14155,7 @@
         <v>2.043374659723468</v>
       </c>
       <c r="E491" t="n">
-        <v>0.03192852973720867</v>
+        <v>1.82937</v>
       </c>
       <c r="F491" t="n">
         <v>-0.236754</v>
@@ -14183,7 +14183,7 @@
         <v>2.046516552583927</v>
       </c>
       <c r="E492" t="n">
-        <v>0.04251622057858186</v>
+        <v>2.436</v>
       </c>
       <c r="F492" t="n">
         <v>-0.00386315</v>
@@ -14211,7 +14211,7 @@
         <v>2.044727365689617</v>
       </c>
       <c r="E493" t="n">
-        <v>0.05439196440792688</v>
+        <v>3.11643</v>
       </c>
       <c r="F493" t="n">
         <v>0.0167206</v>
@@ -14239,7 +14239,7 @@
         <v>2.037508282191756</v>
       </c>
       <c r="E494" t="n">
-        <v>0.06390889575320156</v>
+        <v>3.66171</v>
       </c>
       <c r="F494" t="n">
         <v>0.191874</v>
@@ -14267,7 +14267,7 @@
         <v>2.01949993810349</v>
       </c>
       <c r="E495" t="n">
-        <v>0.07532439625879567</v>
+        <v>4.31577</v>
       </c>
       <c r="F495" t="n">
         <v>-0.457244</v>
@@ -14295,7 +14295,7 @@
         <v>2.04296598111667</v>
       </c>
       <c r="E496" t="n">
-        <v>0.08701757864838208</v>
+        <v>4.98574</v>
       </c>
       <c r="F496" t="n">
         <v>-0.329872</v>
@@ -14323,7 +14323,7 @@
         <v>2.011444754399186</v>
       </c>
       <c r="E497" t="n">
-        <v>0.09747716232265889</v>
+        <v>5.58503</v>
       </c>
       <c r="F497" t="n">
         <v>-0.169693</v>
@@ -14351,7 +14351,7 @@
         <v>2.081030994483263</v>
       </c>
       <c r="E498" t="n">
-        <v>0.1061720435902443</v>
+        <v>6.08321</v>
       </c>
       <c r="F498" t="n">
         <v>-0.080988</v>
@@ -14379,7 +14379,7 @@
         <v>2.441089920506821</v>
       </c>
       <c r="E499" t="n">
-        <v>0.00351785073373473</v>
+        <v>0.201558</v>
       </c>
       <c r="F499" t="n">
         <v>0.0774504</v>
@@ -14407,7 +14407,7 @@
         <v>2.429823038824021</v>
       </c>
       <c r="E500" t="n">
-        <v>0.009043929664691697</v>
+        <v>0.5181789999999999</v>
       </c>
       <c r="F500" t="n">
         <v>-0.082027</v>
@@ -14435,7 +14435,7 @@
         <v>2.401332963168581</v>
       </c>
       <c r="E501" t="n">
-        <v>0.01569979512704963</v>
+        <v>0.899532</v>
       </c>
       <c r="F501" t="n">
         <v>0.245013</v>
@@ -14463,7 +14463,7 @@
         <v>2.385481083555265</v>
       </c>
       <c r="E502" t="n">
-        <v>0.022283840290688</v>
+        <v>1.27677</v>
       </c>
       <c r="F502" t="n">
         <v>0.163176</v>
@@ -14491,7 +14491,7 @@
         <v>2.4014329055795</v>
       </c>
       <c r="E503" t="n">
-        <v>0.03126617728607682</v>
+        <v>1.79142</v>
       </c>
       <c r="F503" t="n">
         <v>0.215279</v>
@@ -14519,7 +14519,7 @@
         <v>2.443198722985914</v>
       </c>
       <c r="E504" t="n">
-        <v>0.04193729486569534</v>
+        <v>2.40283</v>
       </c>
       <c r="F504" t="n">
         <v>0.00530533</v>
@@ -14547,7 +14547,7 @@
         <v>2.430555492063491</v>
       </c>
       <c r="E505" t="n">
-        <v>0.08639659050052251</v>
+        <v>4.95016</v>
       </c>
       <c r="F505" t="n">
         <v>-0.193446</v>
@@ -14575,7 +14575,7 @@
         <v>2.424714416173583</v>
       </c>
       <c r="E506" t="n">
-        <v>0.09752306448198635</v>
+        <v>5.58766</v>
       </c>
       <c r="F506" t="n">
         <v>-0.223748</v>
@@ -14603,7 +14603,7 @@
         <v>2.402933623719141</v>
       </c>
       <c r="E507" t="n">
-        <v>0.1065308832844543</v>
+        <v>6.10377</v>
       </c>
       <c r="F507" t="n">
         <v>-0.0914943</v>
@@ -14631,7 +14631,7 @@
         <v>2.391114802764602</v>
       </c>
       <c r="E508" t="n">
-        <v>0.005314963904635732</v>
+        <v>0.304525</v>
       </c>
       <c r="F508" t="n">
         <v>0.0775522</v>
@@ -14659,7 +14659,7 @@
         <v>2.39375646213227</v>
       </c>
       <c r="E509" t="n">
-        <v>0.01493017474009021</v>
+        <v>0.855436</v>
       </c>
       <c r="F509" t="n">
         <v>0.413535</v>
@@ -14687,7 +14687,7 @@
         <v>2.433557067339905</v>
       </c>
       <c r="E510" t="n">
-        <v>0.02653703314487298</v>
+        <v>1.52046</v>
       </c>
       <c r="F510" t="n">
         <v>0.369131</v>
@@ -14715,7 +14715,7 @@
         <v>2.423142587632845</v>
       </c>
       <c r="E511" t="n">
-        <v>0.03588362035515302</v>
+        <v>2.05598</v>
       </c>
       <c r="F511" t="n">
         <v>0.349085</v>
@@ -14743,7 +14743,7 @@
         <v>2.446989987719606</v>
       </c>
       <c r="E512" t="n">
-        <v>0.04829954358799028</v>
+        <v>2.76736</v>
       </c>
       <c r="F512" t="n">
         <v>0.029331</v>
@@ -14771,7 +14771,7 @@
         <v>2.414818833784431</v>
       </c>
       <c r="E513" t="n">
-        <v>0.08163603043278277</v>
+        <v>4.6774</v>
       </c>
       <c r="F513" t="n">
         <v>-0.472629</v>
@@ -14799,7 +14799,7 @@
         <v>2.409614076984113</v>
       </c>
       <c r="E514" t="n">
-        <v>0.09184219229967001</v>
+        <v>5.26217</v>
       </c>
       <c r="F514" t="n">
         <v>-0.152555</v>
@@ -14827,7 +14827,7 @@
         <v>2.366157222164242</v>
       </c>
       <c r="E515" t="n">
-        <v>0.104416242362738</v>
+        <v>5.98261</v>
       </c>
       <c r="F515" t="n">
         <v>-0.170389</v>
@@ -14855,7 +14855,7 @@
         <v>2.353399668564607</v>
       </c>
       <c r="E516" t="n">
-        <v>0.00194211512515669</v>
+        <v>0.111275</v>
       </c>
       <c r="F516" t="n">
         <v>0.0513152</v>
@@ -14883,7 +14883,7 @@
         <v>2.366296684695307</v>
       </c>
       <c r="E517" t="n">
-        <v>0.00774125081758817</v>
+        <v>0.443541</v>
       </c>
       <c r="F517" t="n">
         <v>0.112426</v>
@@ -14911,7 +14911,7 @@
         <v>2.418706265754484</v>
       </c>
       <c r="E518" t="n">
-        <v>0.01962291131309744</v>
+        <v>1.12431</v>
       </c>
       <c r="F518" t="n">
         <v>0.07401149999999999</v>
@@ -14939,7 +14939,7 @@
         <v>2.445516305404648</v>
       </c>
       <c r="E519" t="n">
-        <v>0.0291180260427222</v>
+        <v>1.66834</v>
       </c>
       <c r="F519" t="n">
         <v>0.297</v>
@@ -14967,7 +14967,7 @@
         <v>2.40546669068603</v>
       </c>
       <c r="E520" t="n">
-        <v>0.03919834967054064</v>
+        <v>2.2459</v>
       </c>
       <c r="F520" t="n">
         <v>-0.130885</v>
@@ -14995,7 +14995,7 @@
         <v>2.459640217592809</v>
       </c>
       <c r="E521" t="n">
-        <v>0.06185062896632465</v>
+        <v>3.54378</v>
       </c>
       <c r="F521" t="n">
         <v>0.0112543</v>
@@ -15023,7 +15023,7 @@
         <v>2.344794234042723</v>
       </c>
       <c r="E522" t="n">
-        <v>0.1065657898694942</v>
+        <v>6.10577</v>
       </c>
       <c r="F522" t="n">
         <v>-0.200763</v>
@@ -15051,7 +15051,7 @@
         <v>2.428019769277013</v>
       </c>
       <c r="E523" t="n">
-        <v>0.003432626306359847</v>
+        <v>0.196675</v>
       </c>
       <c r="F523" t="n">
         <v>-0.0462211</v>
@@ -15079,7 +15079,7 @@
         <v>2.411285963961969</v>
       </c>
       <c r="E524" t="n">
-        <v>0.01097278028753323</v>
+        <v>0.628694</v>
       </c>
       <c r="F524" t="n">
         <v>-0.0349884</v>
@@ -15107,7 +15107,7 @@
         <v>2.4764753178661</v>
       </c>
       <c r="E525" t="n">
-        <v>0.0222210084376162</v>
+        <v>1.27317</v>
       </c>
       <c r="F525" t="n">
         <v>-0.162325</v>
@@ -15135,7 +15135,7 @@
         <v>2.40007708209549</v>
       </c>
       <c r="E526" t="n">
-        <v>0.07791621019800725</v>
+        <v>4.46427</v>
       </c>
       <c r="F526" t="n">
         <v>-0.322069</v>
@@ -15163,7 +15163,7 @@
         <v>2.457687937879828</v>
       </c>
       <c r="E527" t="n">
-        <v>0.08822866261634095</v>
+        <v>5.05513</v>
       </c>
       <c r="F527" t="n">
         <v>-0.125249</v>
@@ -15191,7 +15191,7 @@
         <v>2.431347363089034</v>
       </c>
       <c r="E528" t="n">
-        <v>0.1022438310427806</v>
+        <v>5.85814</v>
       </c>
       <c r="F528" t="n">
         <v>-0.050524</v>
@@ -15219,7 +15219,7 @@
         <v>2.429131532050087</v>
       </c>
       <c r="E529" t="n">
-        <v>0.1074393271601173</v>
+        <v>6.15582</v>
       </c>
       <c r="F529" t="n">
         <v>0.239287</v>

</xml_diff>

<commit_message>
Upd correct mistake in pol
</commit_message>
<xml_diff>
--- a/Raw_Data/DVCS_data/DVCSoutput/5_ALL_PusMstKs.xlsx
+++ b/Raw_Data/DVCS_data/DVCSoutput/5_ALL_PusMstKs.xlsx
@@ -445,7 +445,7 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -865,7 +865,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -977,7 +977,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4085,7 +4085,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4141,7 +4141,7 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4197,7 +4197,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4673,7 +4673,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4757,7 +4757,7 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4841,7 +4841,7 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4925,7 +4925,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4953,7 +4953,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -4981,7 +4981,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5233,7 +5233,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5261,7 +5261,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5569,7 +5569,7 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5653,7 +5653,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5765,7 +5765,7 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5821,7 +5821,7 @@
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5849,7 +5849,7 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5933,7 +5933,7 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5961,7 +5961,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -5989,7 +5989,7 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6241,7 +6241,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6325,7 +6325,7 @@
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6353,7 +6353,7 @@
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6409,7 +6409,7 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6465,7 +6465,7 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6493,7 +6493,7 @@
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6549,7 +6549,7 @@
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6605,7 +6605,7 @@
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6661,7 +6661,7 @@
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6745,7 +6745,7 @@
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6773,7 +6773,7 @@
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6801,7 +6801,7 @@
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6829,7 +6829,7 @@
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6857,7 +6857,7 @@
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -6997,7 +6997,7 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7025,7 +7025,7 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7081,7 +7081,7 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7193,7 +7193,7 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7277,7 +7277,7 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7305,7 +7305,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7361,7 +7361,7 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7389,7 +7389,7 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7445,7 +7445,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7473,7 +7473,7 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7501,7 +7501,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7529,7 +7529,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7585,7 +7585,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7613,7 +7613,7 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7697,7 +7697,7 @@
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7753,7 +7753,7 @@
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="H264" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7865,7 +7865,7 @@
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7893,7 +7893,7 @@
       </c>
       <c r="H267" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7921,7 +7921,7 @@
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7949,7 +7949,7 @@
       </c>
       <c r="H269" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="H270" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8005,7 +8005,7 @@
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8033,7 +8033,7 @@
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8061,7 +8061,7 @@
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="H275" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8145,7 +8145,7 @@
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8173,7 +8173,7 @@
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8201,7 +8201,7 @@
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8257,7 +8257,7 @@
       </c>
       <c r="H280" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8313,7 +8313,7 @@
       </c>
       <c r="H282" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8341,7 +8341,7 @@
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8369,7 +8369,7 @@
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8397,7 +8397,7 @@
       </c>
       <c r="H285" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8425,7 +8425,7 @@
       </c>
       <c r="H286" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8453,7 +8453,7 @@
       </c>
       <c r="H287" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="H288" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8509,7 +8509,7 @@
       </c>
       <c r="H289" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="H290" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8565,7 +8565,7 @@
       </c>
       <c r="H291" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8593,7 +8593,7 @@
       </c>
       <c r="H292" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8621,7 +8621,7 @@
       </c>
       <c r="H293" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="H294" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8705,7 +8705,7 @@
       </c>
       <c r="H296" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8733,7 +8733,7 @@
       </c>
       <c r="H297" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="H298" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8789,7 +8789,7 @@
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8817,7 +8817,7 @@
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8845,7 +8845,7 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8873,7 +8873,7 @@
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8901,7 +8901,7 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8929,7 +8929,7 @@
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8957,7 +8957,7 @@
       </c>
       <c r="H305" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -8985,7 +8985,7 @@
       </c>
       <c r="H306" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9013,7 +9013,7 @@
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9041,7 +9041,7 @@
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="H309" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9097,7 +9097,7 @@
       </c>
       <c r="H310" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9125,7 +9125,7 @@
       </c>
       <c r="H311" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9153,7 +9153,7 @@
       </c>
       <c r="H312" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9181,7 +9181,7 @@
       </c>
       <c r="H313" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9209,7 +9209,7 @@
       </c>
       <c r="H314" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9237,7 +9237,7 @@
       </c>
       <c r="H315" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9265,7 +9265,7 @@
       </c>
       <c r="H316" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9293,7 +9293,7 @@
       </c>
       <c r="H317" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9321,7 +9321,7 @@
       </c>
       <c r="H318" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9349,7 +9349,7 @@
       </c>
       <c r="H319" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="H320" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="H321" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9433,7 +9433,7 @@
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="H323" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9489,7 +9489,7 @@
       </c>
       <c r="H324" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9517,7 +9517,7 @@
       </c>
       <c r="H325" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9545,7 +9545,7 @@
       </c>
       <c r="H326" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9573,7 +9573,7 @@
       </c>
       <c r="H327" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9601,7 +9601,7 @@
       </c>
       <c r="H328" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9629,7 +9629,7 @@
       </c>
       <c r="H329" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9657,7 +9657,7 @@
       </c>
       <c r="H330" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9685,7 +9685,7 @@
       </c>
       <c r="H331" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9713,7 +9713,7 @@
       </c>
       <c r="H332" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9741,7 +9741,7 @@
       </c>
       <c r="H333" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9769,7 +9769,7 @@
       </c>
       <c r="H334" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9797,7 +9797,7 @@
       </c>
       <c r="H335" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9825,7 +9825,7 @@
       </c>
       <c r="H336" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9853,7 +9853,7 @@
       </c>
       <c r="H337" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="H338" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="H339" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9937,7 +9937,7 @@
       </c>
       <c r="H340" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9965,7 +9965,7 @@
       </c>
       <c r="H341" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="H342" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="H343" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10049,7 +10049,7 @@
       </c>
       <c r="H344" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10077,7 +10077,7 @@
       </c>
       <c r="H345" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10105,7 +10105,7 @@
       </c>
       <c r="H346" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10133,7 +10133,7 @@
       </c>
       <c r="H347" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10189,7 +10189,7 @@
       </c>
       <c r="H349" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10217,7 +10217,7 @@
       </c>
       <c r="H350" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10245,7 +10245,7 @@
       </c>
       <c r="H351" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10273,7 +10273,7 @@
       </c>
       <c r="H352" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10301,7 +10301,7 @@
       </c>
       <c r="H353" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="H354" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="H355" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10385,7 +10385,7 @@
       </c>
       <c r="H356" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10413,7 +10413,7 @@
       </c>
       <c r="H357" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10441,7 +10441,7 @@
       </c>
       <c r="H358" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10469,7 +10469,7 @@
       </c>
       <c r="H359" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="H360" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10525,7 +10525,7 @@
       </c>
       <c r="H361" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="H362" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10581,7 +10581,7 @@
       </c>
       <c r="H363" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="H364" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10637,7 +10637,7 @@
       </c>
       <c r="H365" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10665,7 +10665,7 @@
       </c>
       <c r="H366" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10693,7 +10693,7 @@
       </c>
       <c r="H367" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10721,7 +10721,7 @@
       </c>
       <c r="H368" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10749,7 +10749,7 @@
       </c>
       <c r="H369" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10777,7 +10777,7 @@
       </c>
       <c r="H370" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10805,7 +10805,7 @@
       </c>
       <c r="H371" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10833,7 +10833,7 @@
       </c>
       <c r="H372" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10861,7 +10861,7 @@
       </c>
       <c r="H373" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10889,7 +10889,7 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10917,7 +10917,7 @@
       </c>
       <c r="H375" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10945,7 +10945,7 @@
       </c>
       <c r="H376" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -10973,7 +10973,7 @@
       </c>
       <c r="H377" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11001,7 +11001,7 @@
       </c>
       <c r="H378" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11029,7 +11029,7 @@
       </c>
       <c r="H379" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11057,7 +11057,7 @@
       </c>
       <c r="H380" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11085,7 +11085,7 @@
       </c>
       <c r="H381" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="H382" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11141,7 +11141,7 @@
       </c>
       <c r="H383" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11169,7 +11169,7 @@
       </c>
       <c r="H384" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11197,7 +11197,7 @@
       </c>
       <c r="H385" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11225,7 +11225,7 @@
       </c>
       <c r="H386" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11253,7 +11253,7 @@
       </c>
       <c r="H387" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11281,7 +11281,7 @@
       </c>
       <c r="H388" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="H389" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11337,7 +11337,7 @@
       </c>
       <c r="H390" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11365,7 +11365,7 @@
       </c>
       <c r="H391" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11393,7 +11393,7 @@
       </c>
       <c r="H392" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11421,7 +11421,7 @@
       </c>
       <c r="H393" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11449,7 +11449,7 @@
       </c>
       <c r="H394" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11477,7 +11477,7 @@
       </c>
       <c r="H395" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11505,7 +11505,7 @@
       </c>
       <c r="H396" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11533,7 +11533,7 @@
       </c>
       <c r="H397" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11561,7 +11561,7 @@
       </c>
       <c r="H398" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11589,7 +11589,7 @@
       </c>
       <c r="H399" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11617,7 +11617,7 @@
       </c>
       <c r="H400" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11645,7 +11645,7 @@
       </c>
       <c r="H401" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11673,7 +11673,7 @@
       </c>
       <c r="H402" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11701,7 +11701,7 @@
       </c>
       <c r="H403" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11729,7 +11729,7 @@
       </c>
       <c r="H404" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11757,7 +11757,7 @@
       </c>
       <c r="H405" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11785,7 +11785,7 @@
       </c>
       <c r="H406" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11813,7 +11813,7 @@
       </c>
       <c r="H407" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11841,7 +11841,7 @@
       </c>
       <c r="H408" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11869,7 +11869,7 @@
       </c>
       <c r="H409" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11897,7 +11897,7 @@
       </c>
       <c r="H410" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11925,7 +11925,7 @@
       </c>
       <c r="H411" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11953,7 +11953,7 @@
       </c>
       <c r="H412" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="H413" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12009,7 +12009,7 @@
       </c>
       <c r="H414" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12037,7 +12037,7 @@
       </c>
       <c r="H415" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12065,7 +12065,7 @@
       </c>
       <c r="H416" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12093,7 +12093,7 @@
       </c>
       <c r="H417" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12121,7 +12121,7 @@
       </c>
       <c r="H418" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12149,7 +12149,7 @@
       </c>
       <c r="H419" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12177,7 +12177,7 @@
       </c>
       <c r="H420" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12205,7 +12205,7 @@
       </c>
       <c r="H421" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12233,7 +12233,7 @@
       </c>
       <c r="H422" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12261,7 +12261,7 @@
       </c>
       <c r="H423" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12289,7 +12289,7 @@
       </c>
       <c r="H424" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12317,7 +12317,7 @@
       </c>
       <c r="H425" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12345,7 +12345,7 @@
       </c>
       <c r="H426" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12373,7 +12373,7 @@
       </c>
       <c r="H427" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12401,7 +12401,7 @@
       </c>
       <c r="H428" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12429,7 +12429,7 @@
       </c>
       <c r="H429" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12457,7 +12457,7 @@
       </c>
       <c r="H430" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12485,7 +12485,7 @@
       </c>
       <c r="H431" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12513,7 +12513,7 @@
       </c>
       <c r="H432" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12541,7 +12541,7 @@
       </c>
       <c r="H433" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12569,7 +12569,7 @@
       </c>
       <c r="H434" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12597,7 +12597,7 @@
       </c>
       <c r="H435" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12625,7 +12625,7 @@
       </c>
       <c r="H436" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12653,7 +12653,7 @@
       </c>
       <c r="H437" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12681,7 +12681,7 @@
       </c>
       <c r="H438" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12709,7 +12709,7 @@
       </c>
       <c r="H439" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12737,7 +12737,7 @@
       </c>
       <c r="H440" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12765,7 +12765,7 @@
       </c>
       <c r="H441" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12793,7 +12793,7 @@
       </c>
       <c r="H442" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12821,7 +12821,7 @@
       </c>
       <c r="H443" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12849,7 +12849,7 @@
       </c>
       <c r="H444" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12877,7 +12877,7 @@
       </c>
       <c r="H445" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12905,7 +12905,7 @@
       </c>
       <c r="H446" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12933,7 +12933,7 @@
       </c>
       <c r="H447" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12961,7 +12961,7 @@
       </c>
       <c r="H448" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -12989,7 +12989,7 @@
       </c>
       <c r="H449" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13017,7 +13017,7 @@
       </c>
       <c r="H450" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13045,7 +13045,7 @@
       </c>
       <c r="H451" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13073,7 +13073,7 @@
       </c>
       <c r="H452" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13101,7 +13101,7 @@
       </c>
       <c r="H453" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13129,7 +13129,7 @@
       </c>
       <c r="H454" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13157,7 +13157,7 @@
       </c>
       <c r="H455" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13185,7 +13185,7 @@
       </c>
       <c r="H456" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13213,7 +13213,7 @@
       </c>
       <c r="H457" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13241,7 +13241,7 @@
       </c>
       <c r="H458" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13269,7 +13269,7 @@
       </c>
       <c r="H459" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13297,7 +13297,7 @@
       </c>
       <c r="H460" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13325,7 +13325,7 @@
       </c>
       <c r="H461" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13353,7 +13353,7 @@
       </c>
       <c r="H462" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13381,7 +13381,7 @@
       </c>
       <c r="H463" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13409,7 +13409,7 @@
       </c>
       <c r="H464" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13437,7 +13437,7 @@
       </c>
       <c r="H465" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13465,7 +13465,7 @@
       </c>
       <c r="H466" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13493,7 +13493,7 @@
       </c>
       <c r="H467" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13521,7 +13521,7 @@
       </c>
       <c r="H468" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13549,7 +13549,7 @@
       </c>
       <c r="H469" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13577,7 +13577,7 @@
       </c>
       <c r="H470" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13605,7 +13605,7 @@
       </c>
       <c r="H471" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13633,7 +13633,7 @@
       </c>
       <c r="H472" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13661,7 +13661,7 @@
       </c>
       <c r="H473" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13689,7 +13689,7 @@
       </c>
       <c r="H474" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13717,7 +13717,7 @@
       </c>
       <c r="H475" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13745,7 +13745,7 @@
       </c>
       <c r="H476" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13773,7 +13773,7 @@
       </c>
       <c r="H477" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13801,7 +13801,7 @@
       </c>
       <c r="H478" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13829,7 +13829,7 @@
       </c>
       <c r="H479" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13857,7 +13857,7 @@
       </c>
       <c r="H480" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13885,7 +13885,7 @@
       </c>
       <c r="H481" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13913,7 +13913,7 @@
       </c>
       <c r="H482" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13941,7 +13941,7 @@
       </c>
       <c r="H483" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13969,7 +13969,7 @@
       </c>
       <c r="H484" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -13997,7 +13997,7 @@
       </c>
       <c r="H485" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14025,7 +14025,7 @@
       </c>
       <c r="H486" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14053,7 +14053,7 @@
       </c>
       <c r="H487" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14081,7 +14081,7 @@
       </c>
       <c r="H488" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14109,7 +14109,7 @@
       </c>
       <c r="H489" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14137,7 +14137,7 @@
       </c>
       <c r="H490" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14165,7 +14165,7 @@
       </c>
       <c r="H491" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14193,7 +14193,7 @@
       </c>
       <c r="H492" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14221,7 +14221,7 @@
       </c>
       <c r="H493" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14249,7 +14249,7 @@
       </c>
       <c r="H494" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14277,7 +14277,7 @@
       </c>
       <c r="H495" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14305,7 +14305,7 @@
       </c>
       <c r="H496" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14333,7 +14333,7 @@
       </c>
       <c r="H497" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14361,7 +14361,7 @@
       </c>
       <c r="H498" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14389,7 +14389,7 @@
       </c>
       <c r="H499" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14417,7 +14417,7 @@
       </c>
       <c r="H500" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14445,7 +14445,7 @@
       </c>
       <c r="H501" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14473,7 +14473,7 @@
       </c>
       <c r="H502" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14501,7 +14501,7 @@
       </c>
       <c r="H503" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14529,7 +14529,7 @@
       </c>
       <c r="H504" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14557,7 +14557,7 @@
       </c>
       <c r="H505" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14585,7 +14585,7 @@
       </c>
       <c r="H506" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14613,7 +14613,7 @@
       </c>
       <c r="H507" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14641,7 +14641,7 @@
       </c>
       <c r="H508" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14669,7 +14669,7 @@
       </c>
       <c r="H509" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14697,7 +14697,7 @@
       </c>
       <c r="H510" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14725,7 +14725,7 @@
       </c>
       <c r="H511" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14753,7 +14753,7 @@
       </c>
       <c r="H512" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14781,7 +14781,7 @@
       </c>
       <c r="H513" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="H514" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14837,7 +14837,7 @@
       </c>
       <c r="H515" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14865,7 +14865,7 @@
       </c>
       <c r="H516" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14893,7 +14893,7 @@
       </c>
       <c r="H517" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14921,7 +14921,7 @@
       </c>
       <c r="H518" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14949,7 +14949,7 @@
       </c>
       <c r="H519" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -14977,7 +14977,7 @@
       </c>
       <c r="H520" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15005,7 +15005,7 @@
       </c>
       <c r="H521" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15033,7 +15033,7 @@
       </c>
       <c r="H522" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15061,7 +15061,7 @@
       </c>
       <c r="H523" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15089,7 +15089,7 @@
       </c>
       <c r="H524" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15117,7 +15117,7 @@
       </c>
       <c r="H525" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15145,7 +15145,7 @@
       </c>
       <c r="H526" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15173,7 +15173,7 @@
       </c>
       <c r="H527" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15201,7 +15201,7 @@
       </c>
       <c r="H528" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
@@ -15229,7 +15229,7 @@
       </c>
       <c r="H529" t="inlineStr">
         <is>
-          <t>LL</t>
+          <t>LU</t>
         </is>
       </c>
     </row>

</xml_diff>